<commit_message>
PlotPanel bugfixes & improvements // Test updates to work with analyse_average_x & PlotPanel
</commit_message>
<xml_diff>
--- a/example data/group/12 mm - Grand Average Group Stepcycles.xlsx
+++ b/example data/group/12 mm - Grand Average Group Stepcycles.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AK26"/>
+  <dimension ref="A1:AZ26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,170 +451,245 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Nose x</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Nose y</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Ear base x</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Ear base y</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Front paw tao x</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Front paw tao y</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Wrist x</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Wrist y</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Elbow x</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Elbow y</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Lower Shoulder x</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Lower Shoulder y</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Upper Shoulder x</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Upper Shoulder y</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Iliac Crest x</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Iliac Crest y</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Hip x</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Hip y</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Knee x</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Knee y</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Ankle x</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>Ankle y</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>Hind paw tao x</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>Hind paw tao y</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>Tail base x</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>Tail base y</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>Tail center x</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>Tail center y</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>Tail tip x</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>Tail tip y</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>Ankle Angle</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>Knee Angle</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>Hip Angle</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>Hind paw tao Velocity</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>Hind paw tao Acceleration</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>Ankle Velocity</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>Ankle Acceleration</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>Knee Velocity</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>Knee Acceleration</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>Hip Velocity</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>Hip Acceleration</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>Iliac Crest Velocity</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>Iliac Crest Acceleration</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>Ankle Angle Velocity</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AV1" s="1" t="inlineStr">
         <is>
           <t>Ankle Angle Acceleration</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AW1" s="1" t="inlineStr">
         <is>
           <t>Knee Angle Velocity</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AX1" s="1" t="inlineStr">
         <is>
           <t>Knee Angle Acceleration</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AY1" s="1" t="inlineStr">
         <is>
           <t>Hip Angle Velocity</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AZ1" s="1" t="inlineStr">
         <is>
           <t>Hip Angle Acceleration</t>
         </is>
@@ -631,105 +706,150 @@
         <v>2.75</v>
       </c>
       <c r="D2" t="n">
+        <v>229.4239729008776</v>
+      </c>
+      <c r="E2" t="n">
         <v>8.004329390559633</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
+        <v>213.9313773060521</v>
+      </c>
+      <c r="G2" t="n">
         <v>16.29720326011062</v>
       </c>
-      <c r="F2" t="n">
+      <c r="H2" t="n">
+        <v>203.1820379673167</v>
+      </c>
+      <c r="I2" t="n">
         <v>1.477278039810506</v>
       </c>
-      <c r="G2" t="n">
+      <c r="J2" t="n">
+        <v>199.7424405517307</v>
+      </c>
+      <c r="K2" t="n">
         <v>3.746493488338825</v>
       </c>
-      <c r="H2" t="n">
+      <c r="L2" t="n">
+        <v>196.0692655955646</v>
+      </c>
+      <c r="M2" t="n">
         <v>12.92844867029934</v>
       </c>
-      <c r="I2" t="n">
+      <c r="N2" t="n">
+        <v>202.7712717546639</v>
+      </c>
+      <c r="O2" t="n">
         <v>17.25368347573788</v>
       </c>
-      <c r="J2" t="n">
+      <c r="P2" t="n">
+        <v>199.1296749165718</v>
+      </c>
+      <c r="Q2" t="n">
         <v>25.02958554748102</v>
       </c>
-      <c r="K2" t="n">
+      <c r="R2" t="n">
+        <v>156.4092625328835</v>
+      </c>
+      <c r="S2" t="n">
         <v>25.89415920541642</v>
       </c>
-      <c r="L2" t="n">
+      <c r="T2" t="n">
+        <v>151.3383008064108</v>
+      </c>
+      <c r="U2" t="n">
         <v>19.32489280159592</v>
       </c>
-      <c r="M2" t="n">
+      <c r="V2" t="n">
+        <v>155.0260239881827</v>
+      </c>
+      <c r="W2" t="n">
         <v>11.64739757564897</v>
       </c>
-      <c r="N2" t="n">
+      <c r="X2" t="n">
+        <v>143.6483168538581</v>
+      </c>
+      <c r="Y2" t="n">
         <v>15.91882266051381</v>
       </c>
-      <c r="O2" t="n">
+      <c r="Z2" t="n">
+        <v>140.9579576118618</v>
+      </c>
+      <c r="AA2" t="n">
         <v>4.590724038739578</v>
       </c>
-      <c r="P2" t="n">
+      <c r="AB2" t="n">
+        <v>138.2184572570713</v>
+      </c>
+      <c r="AC2" t="n">
         <v>19.60643589073884</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="AD2" t="n">
+        <v>106.8047536880518</v>
+      </c>
+      <c r="AE2" t="n">
         <v>32.17900839257747</v>
       </c>
-      <c r="R2" t="n">
+      <c r="AF2" t="n">
+        <v>94.72354048242173</v>
+      </c>
+      <c r="AG2" t="n">
         <v>38.59543893354159</v>
       </c>
-      <c r="S2" t="n">
+      <c r="AH2" t="n">
         <v>82.89483601404314</v>
       </c>
-      <c r="T2" t="n">
+      <c r="AI2" t="n">
         <v>44.15511990793129</v>
       </c>
-      <c r="U2" t="n">
+      <c r="AJ2" t="n">
         <v>117.1057977285986</v>
       </c>
-      <c r="V2" t="n">
+      <c r="AK2" t="n">
         <v>7.710383013419227</v>
       </c>
-      <c r="W2" t="n">
+      <c r="AL2" t="n">
         <v>0.1858914020002312</v>
       </c>
-      <c r="X2" t="n">
+      <c r="AM2" t="n">
         <v>4.461911727562018</v>
       </c>
-      <c r="Y2" t="n">
+      <c r="AN2" t="n">
         <v>-0.2344615783885856</v>
       </c>
-      <c r="Z2" t="n">
+      <c r="AO2" t="n">
         <v>4.540141592634491</v>
       </c>
-      <c r="AA2" t="n">
+      <c r="AP2" t="n">
         <v>-0.230169814106426</v>
       </c>
-      <c r="AB2" t="n">
+      <c r="AQ2" t="n">
         <v>2.143759148340697</v>
       </c>
-      <c r="AC2" t="n">
+      <c r="AR2" t="n">
         <v>0.3075582814132113</v>
       </c>
-      <c r="AD2" t="n">
+      <c r="AS2" t="n">
         <v>1.829335938954182</v>
       </c>
-      <c r="AE2" t="n">
+      <c r="AT2" t="n">
         <v>0.4276934033589976</v>
       </c>
-      <c r="AF2" t="n">
+      <c r="AU2" t="n">
         <v>-10.91204876970458</v>
       </c>
-      <c r="AG2" t="n">
+      <c r="AV2" t="n">
         <v>1.379573367649637</v>
       </c>
-      <c r="AH2" t="n">
+      <c r="AW2" t="n">
         <v>-12.0390644935228</v>
       </c>
-      <c r="AI2" t="n">
+      <c r="AX2" t="n">
         <v>7.226179822440107</v>
       </c>
-      <c r="AJ2" t="n">
+      <c r="AY2" t="n">
         <v>-16.93786126752475</v>
       </c>
-      <c r="AK2" t="n">
+      <c r="AZ2" t="n">
         <v>3.560772279826844</v>
       </c>
     </row>
@@ -744,105 +864,150 @@
         <v>2.75</v>
       </c>
       <c r="D3" t="n">
+        <v>231.3780467983679</v>
+      </c>
+      <c r="E3" t="n">
         <v>8.115004478616914</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
+        <v>215.7249781256872</v>
+      </c>
+      <c r="G3" t="n">
         <v>16.27174691951022</v>
       </c>
-      <c r="F3" t="n">
+      <c r="H3" t="n">
+        <v>203.2590279342435</v>
+      </c>
+      <c r="I3" t="n">
         <v>1.472459617235983</v>
       </c>
-      <c r="G3" t="n">
+      <c r="J3" t="n">
+        <v>199.8683574774587</v>
+      </c>
+      <c r="K3" t="n">
         <v>3.785397482256515</v>
       </c>
-      <c r="H3" t="n">
+      <c r="L3" t="n">
+        <v>197.5134624234328</v>
+      </c>
+      <c r="M3" t="n">
         <v>13.21335092503974</v>
       </c>
-      <c r="I3" t="n">
+      <c r="N3" t="n">
+        <v>204.3515814534316</v>
+      </c>
+      <c r="O3" t="n">
         <v>17.25430116585807</v>
       </c>
-      <c r="J3" t="n">
+      <c r="P3" t="n">
+        <v>200.8162474378627</v>
+      </c>
+      <c r="Q3" t="n">
         <v>24.99614700357964</v>
       </c>
-      <c r="K3" t="n">
+      <c r="R3" t="n">
+        <v>158.7418930539003</v>
+      </c>
+      <c r="S3" t="n">
         <v>25.83034900908774</v>
       </c>
-      <c r="L3" t="n">
+      <c r="T3" t="n">
+        <v>153.9055726840987</v>
+      </c>
+      <c r="U3" t="n">
         <v>19.18547356382329</v>
       </c>
-      <c r="M3" t="n">
+      <c r="V3" t="n">
+        <v>159.5638799329176</v>
+      </c>
+      <c r="W3" t="n">
         <v>13.10347073467065</v>
       </c>
-      <c r="N3" t="n">
+      <c r="X3" t="n">
+        <v>147.9854573277717</v>
+      </c>
+      <c r="Y3" t="n">
         <v>15.23920407531955</v>
       </c>
-      <c r="O3" t="n">
+      <c r="Z3" t="n">
+        <v>149.2639160959433</v>
+      </c>
+      <c r="AA3" t="n">
         <v>4.751166722453231</v>
       </c>
-      <c r="P3" t="n">
+      <c r="AB3" t="n">
+        <v>140.1710892717043</v>
+      </c>
+      <c r="AC3" t="n">
         <v>19.25754310391474</v>
       </c>
-      <c r="Q3" t="n">
+      <c r="AD3" t="n">
+        <v>108.5133991091915</v>
+      </c>
+      <c r="AE3" t="n">
         <v>32.18986666794364</v>
       </c>
-      <c r="R3" t="n">
+      <c r="AF3" t="n">
+        <v>95.40938172780031</v>
+      </c>
+      <c r="AG3" t="n">
         <v>39.92922356788148</v>
       </c>
-      <c r="S3" t="n">
+      <c r="AH3" t="n">
         <v>72.76581555304278</v>
       </c>
-      <c r="T3" t="n">
+      <c r="AI3" t="n">
         <v>38.95224863373178</v>
       </c>
-      <c r="U3" t="n">
+      <c r="AJ3" t="n">
         <v>103.0371004958303</v>
       </c>
-      <c r="V3" t="n">
+      <c r="AK3" t="n">
         <v>7.612573788732503</v>
       </c>
-      <c r="W3" t="n">
+      <c r="AL3" t="n">
         <v>-0.1553114952770525</v>
       </c>
-      <c r="X3" t="n">
+      <c r="AM3" t="n">
         <v>4.206428122013172</v>
       </c>
-      <c r="Y3" t="n">
+      <c r="AN3" t="n">
         <v>-0.01020258464288842</v>
       </c>
-      <c r="Z3" t="n">
+      <c r="AO3" t="n">
         <v>3.984633489703457</v>
       </c>
-      <c r="AA3" t="n">
+      <c r="AP3" t="n">
         <v>-0.3248905670558316</v>
       </c>
-      <c r="AB3" t="n">
+      <c r="AQ3" t="n">
         <v>2.542632046743486</v>
       </c>
-      <c r="AC3" t="n">
+      <c r="AR3" t="n">
         <v>0.05373418436828179</v>
       </c>
-      <c r="AD3" t="n">
+      <c r="AS3" t="n">
         <v>2.308316645047343</v>
       </c>
-      <c r="AE3" t="n">
+      <c r="AT3" t="n">
         <v>0.01037861121462308</v>
       </c>
-      <c r="AF3" t="n">
+      <c r="AU3" t="n">
         <v>-8.683269119635767</v>
       </c>
-      <c r="AG3" t="n">
+      <c r="AV3" t="n">
         <v>3.509121067001453</v>
       </c>
-      <c r="AH3" t="n">
+      <c r="AW3" t="n">
         <v>-1.215715053376648</v>
       </c>
-      <c r="AI3" t="n">
+      <c r="AX3" t="n">
         <v>7.260776330162156</v>
       </c>
-      <c r="AJ3" t="n">
+      <c r="AY3" t="n">
         <v>-10.5993053183903</v>
       </c>
-      <c r="AK3" t="n">
+      <c r="AZ3" t="n">
         <v>3.273191512175471</v>
       </c>
     </row>
@@ -857,105 +1022,150 @@
         <v>2.75</v>
       </c>
       <c r="D4" t="n">
+        <v>234.4598560891253</v>
+      </c>
+      <c r="E4" t="n">
         <v>8.557858027464954</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
+        <v>218.4725158603479</v>
+      </c>
+      <c r="G4" t="n">
         <v>16.48608944940228</v>
       </c>
-      <c r="F4" t="n">
+      <c r="H4" t="n">
+        <v>203.2941561641423</v>
+      </c>
+      <c r="I4" t="n">
         <v>1.536363574629984</v>
       </c>
-      <c r="G4" t="n">
+      <c r="J4" t="n">
+        <v>200.0767946666014</v>
+      </c>
+      <c r="K4" t="n">
         <v>3.844631648232748</v>
       </c>
-      <c r="H4" t="n">
+      <c r="L4" t="n">
+        <v>199.7102086425673</v>
+      </c>
+      <c r="M4" t="n">
         <v>13.5248858877953</v>
       </c>
-      <c r="I4" t="n">
+      <c r="N4" t="n">
+        <v>206.7573251453697</v>
+      </c>
+      <c r="O4" t="n">
         <v>17.31568008449906</v>
       </c>
-      <c r="J4" t="n">
+      <c r="P4" t="n">
+        <v>203.1450408993038</v>
+      </c>
+      <c r="Q4" t="n">
         <v>25.03282727924644</v>
       </c>
-      <c r="K4" t="n">
+      <c r="R4" t="n">
+        <v>162.1086391574102</v>
+      </c>
+      <c r="S4" t="n">
         <v>25.7853516450165</v>
       </c>
-      <c r="L4" t="n">
+      <c r="T4" t="n">
+        <v>157.6674944754188</v>
+      </c>
+      <c r="U4" t="n">
         <v>18.95538424769192</v>
       </c>
-      <c r="M4" t="n">
+      <c r="V4" t="n">
+        <v>164.9024958728899</v>
+      </c>
+      <c r="W4" t="n">
         <v>14.27457078974298</v>
       </c>
-      <c r="N4" t="n">
+      <c r="X4" t="n">
+        <v>154.1699574348774</v>
+      </c>
+      <c r="Y4" t="n">
         <v>12.22642144412859</v>
       </c>
-      <c r="O4" t="n">
+      <c r="Z4" t="n">
+        <v>159.6873653061846</v>
+      </c>
+      <c r="AA4" t="n">
         <v>4.234192050095144</v>
       </c>
-      <c r="P4" t="n">
+      <c r="AB4" t="n">
+        <v>143.0550240772836</v>
+      </c>
+      <c r="AC4" t="n">
         <v>18.98780697626425</v>
       </c>
-      <c r="Q4" t="n">
+      <c r="AD4" t="n">
+        <v>111.0680620826728</v>
+      </c>
+      <c r="AE4" t="n">
         <v>32.59247566791291</v>
       </c>
-      <c r="R4" t="n">
+      <c r="AF4" t="n">
+        <v>85.52517051286732</v>
+      </c>
+      <c r="AG4" t="n">
         <v>44.00331517483326</v>
       </c>
-      <c r="S4" t="n">
+      <c r="AH4" t="n">
         <v>65.40962058410005</v>
       </c>
-      <c r="T4" t="n">
+      <c r="AI4" t="n">
         <v>45.34872580469213</v>
       </c>
-      <c r="U4" t="n">
+      <c r="AJ4" t="n">
         <v>91.42444181342823</v>
       </c>
-      <c r="V4" t="n">
+      <c r="AK4" t="n">
         <v>6.917234103307656</v>
       </c>
-      <c r="W4" t="n">
+      <c r="AL4" t="n">
         <v>-0.3553597481115497</v>
       </c>
-      <c r="X4" t="n">
+      <c r="AM4" t="n">
         <v>4.343013475972715</v>
       </c>
-      <c r="Y4" t="n">
+      <c r="AN4" t="n">
         <v>0.1867519651955742</v>
       </c>
-      <c r="Z4" t="n">
+      <c r="AO4" t="n">
         <v>3.647919622718864</v>
       </c>
-      <c r="AA4" t="n">
+      <c r="AP4" t="n">
         <v>-0.2170039723950924</v>
       </c>
-      <c r="AB4" t="n">
+      <c r="AQ4" t="n">
         <v>2.548950995113833</v>
       </c>
-      <c r="AC4" t="n">
+      <c r="AR4" t="n">
         <v>0.08973085605506634</v>
       </c>
-      <c r="AD4" t="n">
+      <c r="AS4" t="n">
         <v>2.293202629748811</v>
       </c>
-      <c r="AE4" t="n">
+      <c r="AT4" t="n">
         <v>0.1367093982003229</v>
       </c>
-      <c r="AF4" t="n">
+      <c r="AU4" t="n">
         <v>-4.689835501319387</v>
       </c>
-      <c r="AG4" t="n">
+      <c r="AV4" t="n">
         <v>2.656375016355356</v>
       </c>
-      <c r="AH4" t="n">
+      <c r="AW4" t="n">
         <v>4.583665056618607</v>
       </c>
-      <c r="AI4" t="n">
+      <c r="AX4" t="n">
         <v>4.34345466261728</v>
       </c>
-      <c r="AJ4" t="n">
+      <c r="AY4" t="n">
         <v>-6.837101665190501</v>
       </c>
-      <c r="AK4" t="n">
+      <c r="AZ4" t="n">
         <v>3.107759549140114</v>
       </c>
     </row>
@@ -970,105 +1180,150 @@
         <v>2.75</v>
       </c>
       <c r="D5" t="n">
+        <v>236.6139518876448</v>
+      </c>
+      <c r="E5" t="n">
         <v>8.905564639585238</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
+        <v>220.5581911912201</v>
+      </c>
+      <c r="G5" t="n">
         <v>16.57711614108255</v>
       </c>
-      <c r="F5" t="n">
+      <c r="H5" t="n">
+        <v>203.2685120900472</v>
+      </c>
+      <c r="I5" t="n">
         <v>1.499348667496488</v>
       </c>
-      <c r="G5" t="n">
+      <c r="J5" t="n">
+        <v>200.2985394170098</v>
+      </c>
+      <c r="K5" t="n">
         <v>3.977191194574885</v>
       </c>
-      <c r="H5" t="n">
+      <c r="L5" t="n">
+        <v>201.3850172360738</v>
+      </c>
+      <c r="M5" t="n">
         <v>13.60235315688113</v>
       </c>
-      <c r="I5" t="n">
+      <c r="N5" t="n">
+        <v>208.5370492427907</v>
+      </c>
+      <c r="O5" t="n">
         <v>17.33319049185895</v>
       </c>
-      <c r="J5" t="n">
+      <c r="P5" t="n">
+        <v>205.1496586055621</v>
+      </c>
+      <c r="Q5" t="n">
         <v>25.01305468538974</v>
       </c>
-      <c r="K5" t="n">
+      <c r="R5" t="n">
+        <v>164.8414482461645</v>
+      </c>
+      <c r="S5" t="n">
         <v>25.99196197293329</v>
       </c>
-      <c r="L5" t="n">
+      <c r="T5" t="n">
+        <v>160.7558311722803</v>
+      </c>
+      <c r="U5" t="n">
         <v>18.50055954980511</v>
       </c>
-      <c r="M5" t="n">
+      <c r="V5" t="n">
+        <v>168.3041673602787</v>
+      </c>
+      <c r="W5" t="n">
         <v>14.3418548800421</v>
       </c>
-      <c r="N5" t="n">
+      <c r="X5" t="n">
+        <v>159.5035725874259</v>
+      </c>
+      <c r="Y5" t="n">
         <v>9.513294612262268</v>
       </c>
-      <c r="O5" t="n">
+      <c r="Z5" t="n">
+        <v>165.9164347124438</v>
+      </c>
+      <c r="AA5" t="n">
         <v>4.33978831514399</v>
       </c>
-      <c r="P5" t="n">
+      <c r="AB5" t="n">
+        <v>145.6692847482701</v>
+      </c>
+      <c r="AC5" t="n">
         <v>18.93190323038304</v>
       </c>
-      <c r="Q5" t="n">
+      <c r="AD5" t="n">
+        <v>113.4133123105775</v>
+      </c>
+      <c r="AE5" t="n">
         <v>33.26800359901807</v>
       </c>
-      <c r="R5" t="n">
+      <c r="AF5" t="n">
+        <v>93.53675198417605</v>
+      </c>
+      <c r="AG5" t="n">
         <v>44.13246821004449</v>
       </c>
-      <c r="S5" t="n">
+      <c r="AH5" t="n">
         <v>65.924707911848</v>
       </c>
-      <c r="T5" t="n">
+      <c r="AI5" t="n">
         <v>58.69162698961065</v>
       </c>
-      <c r="U5" t="n">
+      <c r="AJ5" t="n">
         <v>91.8500487591547</v>
       </c>
-      <c r="V5" t="n">
+      <c r="AK5" t="n">
         <v>6.341832115295087</v>
       </c>
-      <c r="W5" t="n">
+      <c r="AL5" t="n">
         <v>-0.1604640261924013</v>
       </c>
-      <c r="X5" t="n">
+      <c r="AM5" t="n">
         <v>4.741358524518655</v>
       </c>
-      <c r="Y5" t="n">
+      <c r="AN5" t="n">
         <v>-0.05116553594034588</v>
       </c>
-      <c r="Z5" t="n">
+      <c r="AO5" t="n">
         <v>3.505244026792814</v>
       </c>
-      <c r="AA5" t="n">
+      <c r="AP5" t="n">
         <v>-0.1770771987049293</v>
       </c>
-      <c r="AB5" t="n">
+      <c r="AQ5" t="n">
         <v>2.68359106060461</v>
       </c>
-      <c r="AC5" t="n">
+      <c r="AR5" t="n">
         <v>0.0509992400382437</v>
       </c>
-      <c r="AD5" t="n">
+      <c r="AS5" t="n">
         <v>2.488611860478175</v>
       </c>
-      <c r="AE5" t="n">
+      <c r="AT5" t="n">
         <v>0.1134021696469511</v>
       </c>
-      <c r="AF5" t="n">
+      <c r="AU5" t="n">
         <v>-2.055632300231132</v>
       </c>
-      <c r="AG5" t="n">
+      <c r="AV5" t="n">
         <v>3.294353991664062</v>
       </c>
-      <c r="AH5" t="n">
+      <c r="AW5" t="n">
         <v>4.991973813949917</v>
       </c>
-      <c r="AI5" t="n">
+      <c r="AX5" t="n">
         <v>2.181040148490976</v>
       </c>
-      <c r="AJ5" t="n">
+      <c r="AY5" t="n">
         <v>-4.836169015679535</v>
       </c>
-      <c r="AK5" t="n">
+      <c r="AZ5" t="n">
         <v>1.412147222127178</v>
       </c>
     </row>
@@ -1083,105 +1338,150 @@
         <v>2.75</v>
       </c>
       <c r="D6" t="n">
+        <v>239.4480502351802</v>
+      </c>
+      <c r="E6" t="n">
         <v>8.924422196462649</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
+        <v>223.3816352296383</v>
+      </c>
+      <c r="G6" t="n">
         <v>16.64618093071255</v>
       </c>
-      <c r="F6" t="n">
+      <c r="H6" t="n">
+        <v>203.2222014369694</v>
+      </c>
+      <c r="I6" t="n">
         <v>1.556172100364741</v>
       </c>
-      <c r="G6" t="n">
+      <c r="J6" t="n">
+        <v>200.7780042945916</v>
+      </c>
+      <c r="K6" t="n">
         <v>4.262477962683286</v>
       </c>
-      <c r="H6" t="n">
+      <c r="L6" t="n">
+        <v>203.6100160991047</v>
+      </c>
+      <c r="M6" t="n">
         <v>13.91035867921004</v>
       </c>
-      <c r="I6" t="n">
+      <c r="N6" t="n">
+        <v>211.0935786937146</v>
+      </c>
+      <c r="O6" t="n">
         <v>17.48847961425782</v>
       </c>
-      <c r="J6" t="n">
+      <c r="P6" t="n">
+        <v>207.7025202994651</v>
+      </c>
+      <c r="Q6" t="n">
         <v>25.27073672477236</v>
       </c>
-      <c r="K6" t="n">
+      <c r="R6" t="n">
+        <v>168.4697474570984</v>
+      </c>
+      <c r="S6" t="n">
         <v>26.25833293224903</v>
       </c>
-      <c r="L6" t="n">
+      <c r="T6" t="n">
+        <v>164.64964265519</v>
+      </c>
+      <c r="U6" t="n">
         <v>18.28877824418089</v>
       </c>
-      <c r="M6" t="n">
+      <c r="V6" t="n">
+        <v>173.0156628375358</v>
+      </c>
+      <c r="W6" t="n">
         <v>14.75163182468279</v>
       </c>
-      <c r="N6" t="n">
+      <c r="X6" t="n">
+        <v>166.0682088939856</v>
+      </c>
+      <c r="Y6" t="n">
         <v>7.745246853388796</v>
       </c>
-      <c r="O6" t="n">
+      <c r="Z6" t="n">
+        <v>174.5246322442454</v>
+      </c>
+      <c r="AA6" t="n">
         <v>3.789065746550863</v>
       </c>
-      <c r="P6" t="n">
+      <c r="AB6" t="n">
+        <v>148.9592233448164</v>
+      </c>
+      <c r="AC6" t="n">
         <v>18.65768128253044</v>
       </c>
-      <c r="Q6" t="n">
+      <c r="AD6" t="n">
+        <v>116.690895061755</v>
+      </c>
+      <c r="AE6" t="n">
         <v>33.64041992958556</v>
       </c>
-      <c r="R6" t="n">
+      <c r="AF6" t="n">
+        <v>85.61858052903034</v>
+      </c>
+      <c r="AG6" t="n">
         <v>45.59391863802647</v>
       </c>
-      <c r="S6" t="n">
+      <c r="AH6" t="n">
         <v>67.93635447885663</v>
       </c>
-      <c r="T6" t="n">
+      <c r="AI6" t="n">
         <v>67.64961876179119</v>
       </c>
-      <c r="U6" t="n">
+      <c r="AJ6" t="n">
         <v>87.82222228662741</v>
       </c>
-      <c r="V6" t="n">
+      <c r="AK6" t="n">
         <v>6.18465487838637</v>
       </c>
-      <c r="W6" t="n">
+      <c r="AL6" t="n">
         <v>-0.5535378418070219</v>
       </c>
-      <c r="X6" t="n">
+      <c r="AM6" t="n">
         <v>4.517102516289301</v>
       </c>
-      <c r="Y6" t="n">
+      <c r="AN6" t="n">
         <v>-0.1667785517712855</v>
       </c>
-      <c r="Z6" t="n">
+      <c r="AO6" t="n">
         <v>3.341852054528309</v>
       </c>
-      <c r="AA6" t="n">
+      <c r="AP6" t="n">
         <v>-0.1633330439844903</v>
       </c>
-      <c r="AB6" t="n">
+      <c r="AQ6" t="n">
         <v>2.790472788590913</v>
       </c>
-      <c r="AC6" t="n">
+      <c r="AR6" t="n">
         <v>0.108626358052516</v>
       </c>
-      <c r="AD6" t="n">
+      <c r="AS6" t="n">
         <v>2.591857377519003</v>
       </c>
-      <c r="AE6" t="n">
+      <c r="AT6" t="n">
         <v>0.06142455212613285</v>
       </c>
-      <c r="AF6" t="n">
+      <c r="AU6" t="n">
         <v>2.663171550538071</v>
       </c>
-      <c r="AG6" t="n">
+      <c r="AV6" t="n">
         <v>2.515073679498385</v>
       </c>
-      <c r="AH6" t="n">
+      <c r="AW6" t="n">
         <v>6.160526550128777</v>
       </c>
-      <c r="AI6" t="n">
+      <c r="AX6" t="n">
         <v>1.633640190460815</v>
       </c>
-      <c r="AJ6" t="n">
+      <c r="AY6" t="n">
         <v>-3.427548562935281</v>
       </c>
-      <c r="AK6" t="n">
+      <c r="AZ6" t="n">
         <v>2.134957057412775</v>
       </c>
     </row>
@@ -1196,105 +1496,150 @@
         <v>2.75</v>
       </c>
       <c r="D7" t="n">
+        <v>241.7690757107227</v>
+      </c>
+      <c r="E7" t="n">
         <v>8.997484132753193</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
+        <v>225.6460160228378</v>
+      </c>
+      <c r="G7" t="n">
         <v>16.77866438601879</v>
       </c>
-      <c r="F7" t="n">
+      <c r="H7" t="n">
+        <v>203.5999553846129</v>
+      </c>
+      <c r="I7" t="n">
         <v>1.730406537969053</v>
       </c>
-      <c r="G7" t="n">
+      <c r="J7" t="n">
+        <v>201.643479673575</v>
+      </c>
+      <c r="K7" t="n">
         <v>4.741530384577757</v>
       </c>
-      <c r="H7" t="n">
+      <c r="L7" t="n">
+        <v>205.4343686036185</v>
+      </c>
+      <c r="M7" t="n">
         <v>14.06266723118775</v>
       </c>
-      <c r="I7" t="n">
+      <c r="N7" t="n">
+        <v>213.0145235264555</v>
+      </c>
+      <c r="O7" t="n">
         <v>17.63730911498374</v>
       </c>
-      <c r="J7" t="n">
+      <c r="P7" t="n">
+        <v>209.7790590414764</v>
+      </c>
+      <c r="Q7" t="n">
         <v>25.40870101739328</v>
       </c>
-      <c r="K7" t="n">
+      <c r="R7" t="n">
+        <v>171.3758170181978</v>
+      </c>
+      <c r="S7" t="n">
         <v>26.70013092933817</v>
       </c>
-      <c r="L7" t="n">
+      <c r="T7" t="n">
+        <v>167.9071204459414</v>
+      </c>
+      <c r="U7" t="n">
         <v>18.48326202825452</v>
       </c>
-      <c r="M7" t="n">
+      <c r="V7" t="n">
+        <v>176.3141530202636</v>
+      </c>
+      <c r="W7" t="n">
         <v>15.32002306999044</v>
       </c>
-      <c r="N7" t="n">
+      <c r="X7" t="n">
+        <v>170.8007775722666</v>
+      </c>
+      <c r="Y7" t="n">
         <v>7.238636118300413</v>
       </c>
-      <c r="O7" t="n">
+      <c r="Z7" t="n">
+        <v>179.6086778877475</v>
+      </c>
+      <c r="AA7" t="n">
         <v>3.145779109170246</v>
       </c>
-      <c r="P7" t="n">
+      <c r="AB7" t="n">
+        <v>151.6371013213557</v>
+      </c>
+      <c r="AC7" t="n">
         <v>18.6549851234923</v>
       </c>
-      <c r="Q7" t="n">
+      <c r="AD7" t="n">
+        <v>119.4168329555938</v>
+      </c>
+      <c r="AE7" t="n">
         <v>33.84060420043079</v>
       </c>
-      <c r="R7" t="n">
+      <c r="AF7" t="n">
+        <v>98.94457968572775</v>
+      </c>
+      <c r="AG7" t="n">
         <v>49.74321947030142</v>
       </c>
-      <c r="S7" t="n">
+      <c r="AH7" t="n">
         <v>76.51631892933769</v>
       </c>
-      <c r="T7" t="n">
+      <c r="AI7" t="n">
         <v>74.20762125338776</v>
       </c>
-      <c r="U7" t="n">
+      <c r="AJ7" t="n">
         <v>88.08503701636127</v>
       </c>
-      <c r="V7" t="n">
+      <c r="AK7" t="n">
         <v>5.049062219071894</v>
       </c>
-      <c r="W7" t="n">
+      <c r="AL7" t="n">
         <v>-1.001844962015218</v>
       </c>
-      <c r="X7" t="n">
+      <c r="AM7" t="n">
         <v>3.979590788800667</v>
       </c>
-      <c r="Y7" t="n">
+      <c r="AN7" t="n">
         <v>-0.4481001208859983</v>
       </c>
-      <c r="Z7" t="n">
+      <c r="AO7" t="n">
         <v>3.253949428281038</v>
       </c>
-      <c r="AA7" t="n">
+      <c r="AP7" t="n">
         <v>-0.1306257349379513</v>
       </c>
-      <c r="AB7" t="n">
+      <c r="AQ7" t="n">
         <v>2.769787112871804</v>
       </c>
-      <c r="AC7" t="n">
+      <c r="AR7" t="n">
         <v>-0.05149108932373353</v>
       </c>
-      <c r="AD7" t="n">
+      <c r="AS7" t="n">
         <v>2.57938140672995</v>
       </c>
-      <c r="AE7" t="n">
+      <c r="AT7" t="n">
         <v>-0.02011166396716043</v>
       </c>
-      <c r="AF7" t="n">
+      <c r="AU7" t="n">
         <v>2.457399469900014</v>
       </c>
-      <c r="AG7" t="n">
+      <c r="AV7" t="n">
         <v>-0.08080729772838469</v>
       </c>
-      <c r="AH7" t="n">
+      <c r="AW7" t="n">
         <v>4.807897705977107</v>
       </c>
-      <c r="AI7" t="n">
+      <c r="AX7" t="n">
         <v>0.7264502332299999</v>
       </c>
-      <c r="AJ7" t="n">
+      <c r="AY7" t="n">
         <v>-1.947184962659934</v>
       </c>
-      <c r="AK7" t="n">
+      <c r="AZ7" t="n">
         <v>2.139961671135204</v>
       </c>
     </row>
@@ -1309,105 +1654,150 @@
         <v>2.75</v>
       </c>
       <c r="D8" t="n">
+        <v>244.6555410822232</v>
+      </c>
+      <c r="E8" t="n">
         <v>9.40396751917846</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
+        <v>228.6301796317946</v>
+      </c>
+      <c r="G8" t="n">
         <v>16.85097234468934</v>
       </c>
-      <c r="F8" t="n">
+      <c r="H8" t="n">
+        <v>204.9021465558532</v>
+      </c>
+      <c r="I8" t="n">
         <v>1.843555768330892</v>
       </c>
-      <c r="G8" t="n">
+      <c r="J8" t="n">
+        <v>203.8527771936241</v>
+      </c>
+      <c r="K8" t="n">
         <v>5.116020195873073</v>
       </c>
-      <c r="H8" t="n">
+      <c r="L8" t="n">
+        <v>207.9301173805345</v>
+      </c>
+      <c r="M8" t="n">
         <v>14.30226200861288</v>
       </c>
-      <c r="I8" t="n">
+      <c r="N8" t="n">
+        <v>215.5783003949105</v>
+      </c>
+      <c r="O8" t="n">
         <v>17.69899442686257</v>
       </c>
-      <c r="J8" t="n">
+      <c r="P8" t="n">
+        <v>212.3990224608293</v>
+      </c>
+      <c r="Q8" t="n">
         <v>25.46227629303087</v>
       </c>
-      <c r="K8" t="n">
+      <c r="R8" t="n">
+        <v>174.5919215340986</v>
+      </c>
+      <c r="S8" t="n">
         <v>27.13182547413711</v>
       </c>
-      <c r="L8" t="n">
+      <c r="T8" t="n">
+        <v>171.3946289204537</v>
+      </c>
+      <c r="U8" t="n">
         <v>18.59921208510162</v>
       </c>
-      <c r="M8" t="n">
+      <c r="V8" t="n">
+        <v>180.3821313888469</v>
+      </c>
+      <c r="W8" t="n">
         <v>15.4796837069464</v>
       </c>
-      <c r="N8" t="n">
+      <c r="X8" t="n">
+        <v>175.2654247672845</v>
+      </c>
+      <c r="Y8" t="n">
         <v>6.088654707509571</v>
       </c>
-      <c r="O8" t="n">
+      <c r="Z8" t="n">
+        <v>184.5635089891177</v>
+      </c>
+      <c r="AA8" t="n">
         <v>2.603602409362796</v>
       </c>
-      <c r="P8" t="n">
+      <c r="AB8" t="n">
+        <v>154.7329268768324</v>
+      </c>
+      <c r="AC8" t="n">
         <v>18.79245372528726</v>
       </c>
-      <c r="Q8" t="n">
+      <c r="AD8" t="n">
+        <v>122.1633566820875</v>
+      </c>
+      <c r="AE8" t="n">
         <v>34.31703849887172</v>
       </c>
-      <c r="R8" t="n">
+      <c r="AF8" t="n">
+        <v>115.6264997965901</v>
+      </c>
+      <c r="AG8" t="n">
         <v>47.72552243361237</v>
       </c>
-      <c r="S8" t="n">
+      <c r="AH8" t="n">
         <v>79.21062320854982</v>
       </c>
-      <c r="T8" t="n">
+      <c r="AI8" t="n">
         <v>79.28392877930703</v>
       </c>
-      <c r="U8" t="n">
+      <c r="AJ8" t="n">
         <v>88.49529530772034</v>
       </c>
-      <c r="V8" t="n">
+      <c r="AK8" t="n">
         <v>3.481162651210813</v>
       </c>
-      <c r="W8" t="n">
+      <c r="AL8" t="n">
         <v>-0.9212670491096836</v>
       </c>
-      <c r="X8" t="n">
+      <c r="AM8" t="n">
         <v>2.981649962722834</v>
       </c>
-      <c r="Y8" t="n">
+      <c r="AN8" t="n">
         <v>-0.4949649492054135</v>
       </c>
-      <c r="Z8" t="n">
+      <c r="AO8" t="n">
         <v>2.939323098101514</v>
       </c>
-      <c r="AA8" t="n">
+      <c r="AP8" t="n">
         <v>-0.3061984236358748</v>
       </c>
-      <c r="AB8" t="n">
+      <c r="AQ8" t="n">
         <v>2.463242538431855</v>
       </c>
-      <c r="AC8" t="n">
+      <c r="AR8" t="n">
         <v>-0.1163837229106445</v>
       </c>
-      <c r="AD8" t="n">
+      <c r="AS8" t="n">
         <v>2.416413536308504</v>
       </c>
-      <c r="AE8" t="n">
+      <c r="AT8" t="n">
         <v>-0.08423162478927446</v>
       </c>
-      <c r="AF8" t="n">
+      <c r="AU8" t="n">
         <v>-0.346037740835804</v>
       </c>
-      <c r="AG8" t="n">
+      <c r="AV8" t="n">
         <v>-0.7740379287433165</v>
       </c>
-      <c r="AH8" t="n">
+      <c r="AW8" t="n">
         <v>3.429941684262592</v>
       </c>
-      <c r="AI8" t="n">
+      <c r="AX8" t="n">
         <v>-0.7919463146482308</v>
       </c>
-      <c r="AJ8" t="n">
+      <c r="AY8" t="n">
         <v>-0.4140071806781604</v>
       </c>
-      <c r="AK8" t="n">
+      <c r="AZ8" t="n">
         <v>0.9737279318655609</v>
       </c>
     </row>
@@ -1422,105 +1812,150 @@
         <v>2.75</v>
       </c>
       <c r="D9" t="n">
+        <v>246.9720305756052</v>
+      </c>
+      <c r="E9" t="n">
         <v>9.564908007357985</v>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
+        <v>231.0446231923205</v>
+      </c>
+      <c r="G9" t="n">
         <v>16.96119409926395</v>
       </c>
-      <c r="F9" t="n">
+      <c r="H9" t="n">
+        <v>207.4565446123163</v>
+      </c>
+      <c r="I9" t="n">
         <v>2.253675291724241</v>
       </c>
-      <c r="G9" t="n">
+      <c r="J9" t="n">
+        <v>207.4178344814489</v>
+      </c>
+      <c r="K9" t="n">
         <v>5.712564279001657</v>
       </c>
-      <c r="H9" t="n">
+      <c r="L9" t="n">
+        <v>210.4239310778625</v>
+      </c>
+      <c r="M9" t="n">
         <v>14.76068682704411</v>
       </c>
-      <c r="I9" t="n">
+      <c r="N9" t="n">
+        <v>218.0304859546905</v>
+      </c>
+      <c r="O9" t="n">
         <v>18.04386588698583</v>
       </c>
-      <c r="J9" t="n">
+      <c r="P9" t="n">
+        <v>214.8074582113442</v>
+      </c>
+      <c r="Q9" t="n">
         <v>25.5641427445919</v>
       </c>
-      <c r="K9" t="n">
+      <c r="R9" t="n">
+        <v>176.9620057116164</v>
+      </c>
+      <c r="S9" t="n">
         <v>27.11334676607281</v>
       </c>
-      <c r="L9" t="n">
+      <c r="T9" t="n">
+        <v>173.5482096672058</v>
+      </c>
+      <c r="U9" t="n">
         <v>18.75657003822056</v>
       </c>
-      <c r="M9" t="n">
+      <c r="V9" t="n">
+        <v>182.8528944059467</v>
+      </c>
+      <c r="W9" t="n">
         <v>15.3583360901961</v>
       </c>
-      <c r="N9" t="n">
+      <c r="X9" t="n">
+        <v>177.0130231025371</v>
+      </c>
+      <c r="Y9" t="n">
         <v>5.76896836571659</v>
       </c>
-      <c r="O9" t="n">
+      <c r="Z9" t="n">
+        <v>186.2069294385031</v>
+      </c>
+      <c r="AA9" t="n">
         <v>2.302750797136454</v>
       </c>
-      <c r="P9" t="n">
+      <c r="AB9" t="n">
+        <v>157.0356528598366</v>
+      </c>
+      <c r="AC9" t="n">
         <v>18.89927353419311</v>
       </c>
-      <c r="Q9" t="n">
+      <c r="AD9" t="n">
+        <v>124.6680889146548</v>
+      </c>
+      <c r="AE9" t="n">
         <v>34.45352358175508</v>
       </c>
-      <c r="R9" t="n">
+      <c r="AF9" t="n">
+        <v>92.68433077538266</v>
+      </c>
+      <c r="AG9" t="n">
         <v>52.15474231868771</v>
       </c>
-      <c r="S9" t="n">
+      <c r="AH9" t="n">
         <v>77.88635729388182</v>
       </c>
-      <c r="T9" t="n">
+      <c r="AI9" t="n">
         <v>78.28150686827325</v>
       </c>
-      <c r="U9" t="n">
+      <c r="AJ9" t="n">
         <v>87.7891989303596</v>
       </c>
-      <c r="V9" t="n">
+      <c r="AK9" t="n">
         <v>2.834915057987188</v>
       </c>
-      <c r="W9" t="n">
+      <c r="AL9" t="n">
         <v>-0.3518504348207021</v>
       </c>
-      <c r="X9" t="n">
+      <c r="AM9" t="n">
         <v>2.457682798940239</v>
       </c>
-      <c r="Y9" t="n">
+      <c r="AN9" t="n">
         <v>-0.01323488375819265</v>
       </c>
-      <c r="Z9" t="n">
+      <c r="AO9" t="n">
         <v>2.413350850977795</v>
       </c>
-      <c r="AA9" t="n">
+      <c r="AP9" t="n">
         <v>-0.214350709678432</v>
       </c>
-      <c r="AB9" t="n">
+      <c r="AQ9" t="n">
         <v>2.274074135942664</v>
       </c>
-      <c r="AC9" t="n">
+      <c r="AR9" t="n">
         <v>0.0522507949078365</v>
       </c>
-      <c r="AD9" t="n">
+      <c r="AS9" t="n">
         <v>2.197427466406045</v>
       </c>
-      <c r="AE9" t="n">
+      <c r="AT9" t="n">
         <v>-0.02962342390777132</v>
       </c>
-      <c r="AF9" t="n">
+      <c r="AU9" t="n">
         <v>-1.249855123160946</v>
       </c>
-      <c r="AG9" t="n">
+      <c r="AV9" t="n">
         <v>0.3733082077126706</v>
       </c>
-      <c r="AH9" t="n">
+      <c r="AW9" t="n">
         <v>2.641215592848413</v>
       </c>
-      <c r="AI9" t="n">
+      <c r="AX9" t="n">
         <v>0.5375696544351183</v>
       </c>
-      <c r="AJ9" t="n">
+      <c r="AY9" t="n">
         <v>0.02928536547522187</v>
       </c>
-      <c r="AK9" t="n">
+      <c r="AZ9" t="n">
         <v>1.637398815837257</v>
       </c>
     </row>
@@ -1535,105 +1970,150 @@
         <v>2.75</v>
       </c>
       <c r="D10" t="n">
+        <v>249.4789765976</v>
+      </c>
+      <c r="E10" t="n">
         <v>9.979577436514781</v>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
+        <v>233.9529916327051</v>
+      </c>
+      <c r="G10" t="n">
         <v>17.19350831728455</v>
       </c>
-      <c r="F10" t="n">
+      <c r="H10" t="n">
+        <v>213.1717548302725</v>
+      </c>
+      <c r="I10" t="n">
         <v>2.858117455286338</v>
       </c>
-      <c r="G10" t="n">
+      <c r="J10" t="n">
+        <v>213.5317126064436</v>
+      </c>
+      <c r="K10" t="n">
         <v>6.297658183050499</v>
       </c>
-      <c r="H10" t="n">
+      <c r="L10" t="n">
+        <v>213.2384613896093</v>
+      </c>
+      <c r="M10" t="n">
         <v>14.88822284319722</v>
       </c>
-      <c r="I10" t="n">
+      <c r="N10" t="n">
+        <v>220.9400613257226</v>
+      </c>
+      <c r="O10" t="n">
         <v>18.3046300360497</v>
       </c>
-      <c r="J10" t="n">
+      <c r="P10" t="n">
+        <v>217.7202526559221</v>
+      </c>
+      <c r="Q10" t="n">
         <v>25.78048469327021</v>
       </c>
-      <c r="K10" t="n">
+      <c r="R10" t="n">
+        <v>179.480858178849</v>
+      </c>
+      <c r="S10" t="n">
         <v>27.00972100521656</v>
       </c>
-      <c r="L10" t="n">
+      <c r="T10" t="n">
+        <v>176.1763497870019</v>
+      </c>
+      <c r="U10" t="n">
         <v>18.57234078941616</v>
       </c>
-      <c r="M10" t="n">
+      <c r="V10" t="n">
+        <v>185.2604863914192</v>
+      </c>
+      <c r="W10" t="n">
         <v>15.08936154926922</v>
       </c>
-      <c r="N10" t="n">
+      <c r="X10" t="n">
+        <v>179.3978817074012</v>
+      </c>
+      <c r="Y10" t="n">
         <v>4.97184256289867</v>
       </c>
-      <c r="O10" t="n">
+      <c r="Z10" t="n">
+        <v>188.9841493139875</v>
+      </c>
+      <c r="AA10" t="n">
         <v>2.433703300800728</v>
       </c>
-      <c r="P10" t="n">
+      <c r="AB10" t="n">
+        <v>159.3395315586252</v>
+      </c>
+      <c r="AC10" t="n">
         <v>19.04103502314141</v>
       </c>
-      <c r="Q10" t="n">
+      <c r="AD10" t="n">
+        <v>127.1209929851775</v>
+      </c>
+      <c r="AE10" t="n">
         <v>34.39513022172536</v>
       </c>
-      <c r="R10" t="n">
+      <c r="AF10" t="n">
+        <v>94.77397171740836</v>
+      </c>
+      <c r="AG10" t="n">
         <v>51.92656068937153</v>
       </c>
-      <c r="S10" t="n">
+      <c r="AH10" t="n">
         <v>74.55019816200236</v>
       </c>
-      <c r="T10" t="n">
+      <c r="AI10" t="n">
         <v>80.9567047224516</v>
       </c>
-      <c r="U10" t="n">
+      <c r="AJ10" t="n">
         <v>89.55444459320867</v>
       </c>
-      <c r="V10" t="n">
+      <c r="AK10" t="n">
         <v>2.663237976689709</v>
       </c>
-      <c r="W10" t="n">
+      <c r="AL10" t="n">
         <v>-0.2324973754849006</v>
       </c>
-      <c r="X10" t="n">
+      <c r="AM10" t="n">
         <v>2.467764036875243</v>
       </c>
-      <c r="Y10" t="n">
+      <c r="AN10" t="n">
         <v>0.05003634496783549</v>
       </c>
-      <c r="Z10" t="n">
+      <c r="AO10" t="n">
         <v>2.217105665105457</v>
       </c>
-      <c r="AA10" t="n">
+      <c r="AP10" t="n">
         <v>-0.08246075388387562</v>
       </c>
-      <c r="AB10" t="n">
+      <c r="AQ10" t="n">
         <v>2.199999597055693</v>
       </c>
-      <c r="AC10" t="n">
+      <c r="AR10" t="n">
         <v>-0.03935581614785297</v>
       </c>
-      <c r="AD10" t="n">
+      <c r="AS10" t="n">
         <v>2.140268577751538</v>
       </c>
-      <c r="AE10" t="n">
+      <c r="AT10" t="n">
         <v>-0.06349150170671151</v>
       </c>
-      <c r="AF10" t="n">
+      <c r="AU10" t="n">
         <v>-0.8653587319811358</v>
       </c>
-      <c r="AG10" t="n">
+      <c r="AV10" t="n">
         <v>1.833185546003302</v>
       </c>
-      <c r="AH10" t="n">
+      <c r="AW10" t="n">
         <v>2.883103782795259</v>
       </c>
-      <c r="AI10" t="n">
+      <c r="AX10" t="n">
         <v>-0.4820863496148319</v>
       </c>
-      <c r="AJ10" t="n">
+      <c r="AY10" t="n">
         <v>0.7422908997191847</v>
       </c>
-      <c r="AK10" t="n">
+      <c r="AZ10" t="n">
         <v>0.3278739397855405</v>
       </c>
     </row>
@@ -1648,105 +2128,150 @@
         <v>2.75</v>
       </c>
       <c r="D11" t="n">
+        <v>251.824220510345</v>
+      </c>
+      <c r="E11" t="n">
         <v>9.824029097320338</v>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
+        <v>236.5354888405361</v>
+      </c>
+      <c r="G11" t="n">
         <v>17.12415776354201</v>
       </c>
-      <c r="F11" t="n">
+      <c r="H11" t="n">
+        <v>218.8766473573996</v>
+      </c>
+      <c r="I11" t="n">
         <v>3.522590204333577</v>
       </c>
-      <c r="G11" t="n">
+      <c r="J11" t="n">
+        <v>217.8722942129095</v>
+      </c>
+      <c r="K11" t="n">
         <v>6.557471701439391</v>
       </c>
-      <c r="H11" t="n">
+      <c r="L11" t="n">
+        <v>216.3329682451614</v>
+      </c>
+      <c r="M11" t="n">
         <v>14.23086477509627</v>
       </c>
-      <c r="I11" t="n">
+      <c r="N11" t="n">
+        <v>223.7860431907871</v>
+      </c>
+      <c r="O11" t="n">
         <v>18.09579598988202</v>
       </c>
-      <c r="J11" t="n">
+      <c r="P11" t="n">
+        <v>220.3339553048425</v>
+      </c>
+      <c r="Q11" t="n">
         <v>25.53930806775465</v>
       </c>
-      <c r="K11" t="n">
+      <c r="R11" t="n">
+        <v>181.715591452646</v>
+      </c>
+      <c r="S11" t="n">
         <v>26.78075800550745</v>
       </c>
-      <c r="L11" t="n">
+      <c r="T11" t="n">
+        <v>178.4680694130296</v>
+      </c>
+      <c r="U11" t="n">
         <v>18.32084233033741</v>
       </c>
-      <c r="M11" t="n">
+      <c r="V11" t="n">
+        <v>187.6704080730465</v>
+      </c>
+      <c r="W11" t="n">
         <v>14.87732762140585</v>
       </c>
-      <c r="N11" t="n">
+      <c r="X11" t="n">
+        <v>182.00521722753</v>
+      </c>
+      <c r="Y11" t="n">
         <v>4.421947188411201</v>
       </c>
-      <c r="O11" t="n">
+      <c r="Z11" t="n">
+        <v>191.6165289303935</v>
+      </c>
+      <c r="AA11" t="n">
         <v>2.191974423455852</v>
       </c>
-      <c r="P11" t="n">
+      <c r="AB11" t="n">
+        <v>161.7030029178511</v>
+      </c>
+      <c r="AC11" t="n">
         <v>18.8249112866449</v>
       </c>
-      <c r="Q11" t="n">
+      <c r="AD11" t="n">
+        <v>129.4188807196651</v>
+      </c>
+      <c r="AE11" t="n">
         <v>33.96712482398284</v>
       </c>
-      <c r="R11" t="n">
+      <c r="AF11" t="n">
+        <v>96.75238815182489</v>
+      </c>
+      <c r="AG11" t="n">
         <v>51.27770968362795</v>
       </c>
-      <c r="S11" t="n">
+      <c r="AH11" t="n">
         <v>74.52969651569633</v>
       </c>
-      <c r="T11" t="n">
+      <c r="AI11" t="n">
         <v>82.23427451332618</v>
       </c>
-      <c r="U11" t="n">
+      <c r="AJ11" t="n">
         <v>89.70236154873756</v>
       </c>
-      <c r="V11" t="n">
+      <c r="AK11" t="n">
         <v>2.354099162926911</v>
       </c>
-      <c r="W11" t="n">
+      <c r="AL11" t="n">
         <v>-0.4759702382358246</v>
       </c>
-      <c r="X11" t="n">
+      <c r="AM11" t="n">
         <v>2.456142610691964</v>
       </c>
-      <c r="Y11" t="n">
+      <c r="AN11" t="n">
         <v>-0.3284844100898057</v>
       </c>
-      <c r="Z11" t="n">
+      <c r="AO11" t="n">
         <v>2.228717558772852</v>
       </c>
-      <c r="AA11" t="n">
+      <c r="AP11" t="n">
         <v>-0.08443207182782934</v>
       </c>
-      <c r="AB11" t="n">
+      <c r="AQ11" t="n">
         <v>2.167298523246819</v>
       </c>
-      <c r="AC11" t="n">
+      <c r="AR11" t="n">
         <v>-0.02085310770264696</v>
       </c>
-      <c r="AD11" t="n">
+      <c r="AS11" t="n">
         <v>2.092075390173188</v>
       </c>
-      <c r="AE11" t="n">
+      <c r="AT11" t="n">
         <v>0.127994031348126</v>
       </c>
-      <c r="AF11" t="n">
+      <c r="AU11" t="n">
         <v>1.465248355693126</v>
       </c>
-      <c r="AG11" t="n">
+      <c r="AV11" t="n">
         <v>0.6626511874860815</v>
       </c>
-      <c r="AH11" t="n">
+      <c r="AW11" t="n">
         <v>1.583431083626601</v>
       </c>
-      <c r="AI11" t="n">
+      <c r="AX11" t="n">
         <v>-1.295976400554768</v>
       </c>
-      <c r="AJ11" t="n">
+      <c r="AY11" t="n">
         <v>0.6956586588337832</v>
       </c>
-      <c r="AK11" t="n">
+      <c r="AZ11" t="n">
         <v>-0.05023571617528597</v>
       </c>
     </row>
@@ -1761,105 +2286,150 @@
         <v>2.75</v>
       </c>
       <c r="D12" t="n">
+        <v>253.7726046900588</v>
+      </c>
+      <c r="E12" t="n">
         <v>9.000799503732239</v>
       </c>
-      <c r="E12" t="n">
+      <c r="F12" t="n">
+        <v>239.0515076353195</v>
+      </c>
+      <c r="G12" t="n">
         <v>16.85586043283449</v>
       </c>
-      <c r="F12" t="n">
+      <c r="H12" t="n">
+        <v>222.9516744190919</v>
+      </c>
+      <c r="I12" t="n">
         <v>3.63014234718701</v>
       </c>
-      <c r="G12" t="n">
+      <c r="J12" t="n">
+        <v>221.512571294257</v>
+      </c>
+      <c r="K12" t="n">
         <v>6.733403983691058</v>
       </c>
-      <c r="H12" t="n">
+      <c r="L12" t="n">
+        <v>219.0883626329138</v>
+      </c>
+      <c r="M12" t="n">
         <v>13.81123826858845</v>
       </c>
-      <c r="I12" t="n">
+      <c r="N12" t="n">
+        <v>226.3854415704173</v>
+      </c>
+      <c r="O12" t="n">
         <v>17.77622006463666</v>
       </c>
-      <c r="J12" t="n">
+      <c r="P12" t="n">
+        <v>222.9704763026948</v>
+      </c>
+      <c r="Q12" t="n">
         <v>25.26136391551782</v>
       </c>
-      <c r="K12" t="n">
+      <c r="R12" t="n">
+        <v>184.1051274157585</v>
+      </c>
+      <c r="S12" t="n">
         <v>26.91745927147832</v>
       </c>
-      <c r="L12" t="n">
+      <c r="T12" t="n">
+        <v>180.7647306868371</v>
+      </c>
+      <c r="U12" t="n">
         <v>18.42434085007255</v>
       </c>
-      <c r="M12" t="n">
+      <c r="V12" t="n">
+        <v>189.9520813996065</v>
+      </c>
+      <c r="W12" t="n">
         <v>14.80711199713092</v>
       </c>
-      <c r="N12" t="n">
+      <c r="X12" t="n">
+        <v>184.3283706523002</v>
+      </c>
+      <c r="Y12" t="n">
         <v>4.446132470529975</v>
       </c>
-      <c r="O12" t="n">
+      <c r="Z12" t="n">
+        <v>193.7204517371266</v>
+      </c>
+      <c r="AA12" t="n">
         <v>1.980122099531456</v>
       </c>
-      <c r="P12" t="n">
+      <c r="AB12" t="n">
+        <v>164.1809411082707</v>
+      </c>
+      <c r="AC12" t="n">
         <v>19.14707312347196</v>
       </c>
-      <c r="Q12" t="n">
+      <c r="AD12" t="n">
+        <v>131.629083765314</v>
+      </c>
+      <c r="AE12" t="n">
         <v>34.05700845921294</v>
       </c>
-      <c r="R12" t="n">
+      <c r="AF12" t="n">
+        <v>98.80120509059716</v>
+      </c>
+      <c r="AG12" t="n">
         <v>51.02770362339967</v>
       </c>
-      <c r="S12" t="n">
+      <c r="AH12" t="n">
         <v>76.10100827277101</v>
       </c>
-      <c r="T12" t="n">
+      <c r="AI12" t="n">
         <v>83.34944534467175</v>
       </c>
-      <c r="U12" t="n">
+      <c r="AJ12" t="n">
         <v>90.34245256405242</v>
       </c>
-      <c r="V12" t="n">
+      <c r="AK12" t="n">
         <v>1.692077876828239</v>
       </c>
-      <c r="W12" t="n">
+      <c r="AL12" t="n">
         <v>-0.6861466042538922</v>
       </c>
-      <c r="X12" t="n">
+      <c r="AM12" t="n">
         <v>1.902349536300551</v>
       </c>
-      <c r="Y12" t="n">
+      <c r="AN12" t="n">
         <v>-0.6347316588070362</v>
       </c>
-      <c r="Z12" t="n">
+      <c r="AO12" t="n">
         <v>2.043348719887697</v>
       </c>
-      <c r="AA12" t="n">
+      <c r="AP12" t="n">
         <v>-0.2867382680270673</v>
       </c>
-      <c r="AB12" t="n">
+      <c r="AQ12" t="n">
         <v>2.135355041382162</v>
       </c>
-      <c r="AC12" t="n">
+      <c r="AR12" t="n">
         <v>-0.1481190640875644</v>
       </c>
-      <c r="AD12" t="n">
+      <c r="AS12" t="n">
         <v>2.321799088877143</v>
       </c>
-      <c r="AE12" t="n">
+      <c r="AT12" t="n">
         <v>-0.07885540208072445</v>
       </c>
-      <c r="AF12" t="n">
+      <c r="AU12" t="n">
         <v>1.454995117316851</v>
       </c>
-      <c r="AG12" t="n">
+      <c r="AV12" t="n">
         <v>-0.573978914586827</v>
       </c>
-      <c r="AH12" t="n">
+      <c r="AW12" t="n">
         <v>0.3476507306618587</v>
       </c>
-      <c r="AI12" t="n">
+      <c r="AX12" t="n">
         <v>-1.484279685179177</v>
       </c>
-      <c r="AJ12" t="n">
+      <c r="AY12" t="n">
         <v>0.6773384806412777</v>
       </c>
-      <c r="AK12" t="n">
+      <c r="AZ12" t="n">
         <v>0.4667306241282136</v>
       </c>
     </row>
@@ -1874,105 +2444,150 @@
         <v>2.75</v>
       </c>
       <c r="D13" t="n">
+        <v>254.2888691397846</v>
+      </c>
+      <c r="E13" t="n">
         <v>8.332313713452498</v>
       </c>
-      <c r="E13" t="n">
+      <c r="F13" t="n">
+        <v>241.4728772978411</v>
+      </c>
+      <c r="G13" t="n">
         <v>16.36364138718193</v>
       </c>
-      <c r="F13" t="n">
+      <c r="H13" t="n">
+        <v>225.9964369290264</v>
+      </c>
+      <c r="I13" t="n">
         <v>3.485817266694199</v>
       </c>
-      <c r="G13" t="n">
+      <c r="J13" t="n">
+        <v>224.4685523898889</v>
+      </c>
+      <c r="K13" t="n">
         <v>6.604202419308066</v>
       </c>
-      <c r="H13" t="n">
+      <c r="L13" t="n">
+        <v>221.4002577125604</v>
+      </c>
+      <c r="M13" t="n">
         <v>13.44987077915922</v>
       </c>
-      <c r="I13" t="n">
+      <c r="N13" t="n">
+        <v>228.8670160246234</v>
+      </c>
+      <c r="O13" t="n">
         <v>17.49586179746804</v>
       </c>
-      <c r="J13" t="n">
+      <c r="P13" t="n">
+        <v>225.5358022155491</v>
+      </c>
+      <c r="Q13" t="n">
         <v>25.06072538118837</v>
       </c>
-      <c r="K13" t="n">
+      <c r="R13" t="n">
+        <v>186.5973668740996</v>
+      </c>
+      <c r="S13" t="n">
         <v>26.91073705118599</v>
       </c>
-      <c r="L13" t="n">
+      <c r="T13" t="n">
+        <v>182.9408079174394</v>
+      </c>
+      <c r="U13" t="n">
         <v>18.50799668765237</v>
       </c>
-      <c r="M13" t="n">
+      <c r="V13" t="n">
+        <v>191.9555831462779</v>
+      </c>
+      <c r="W13" t="n">
         <v>14.46357686468895</v>
       </c>
-      <c r="N13" t="n">
+      <c r="X13" t="n">
+        <v>185.8106262294959</v>
+      </c>
+      <c r="Y13" t="n">
         <v>4.733166796095825</v>
       </c>
-      <c r="O13" t="n">
+      <c r="Z13" t="n">
+        <v>195.0163442192348</v>
+      </c>
+      <c r="AA13" t="n">
         <v>1.65338685326542</v>
       </c>
-      <c r="P13" t="n">
+      <c r="AB13" t="n">
+        <v>166.5314484149852</v>
+      </c>
+      <c r="AC13" t="n">
         <v>19.38558504091087</v>
       </c>
-      <c r="Q13" t="n">
+      <c r="AD13" t="n">
+        <v>134.0429168220953</v>
+      </c>
+      <c r="AE13" t="n">
         <v>33.6339110178305</v>
       </c>
-      <c r="R13" t="n">
+      <c r="AF13" t="n">
+        <v>101.112026187545</v>
+      </c>
+      <c r="AG13" t="n">
         <v>50.53347154712001</v>
       </c>
-      <c r="S13" t="n">
+      <c r="AH13" t="n">
         <v>76.09496461932099</v>
       </c>
-      <c r="T13" t="n">
+      <c r="AI13" t="n">
         <v>82.41418715020134</v>
       </c>
-      <c r="U13" t="n">
+      <c r="AJ13" t="n">
         <v>91.043797336512</v>
       </c>
-      <c r="V13" t="n">
+      <c r="AK13" t="n">
         <v>0.9218461547337554</v>
       </c>
-      <c r="W13" t="n">
+      <c r="AL13" t="n">
         <v>-0.6834739488912801</v>
       </c>
-      <c r="X13" t="n">
+      <c r="AM13" t="n">
         <v>1.196524141528082</v>
       </c>
-      <c r="Y13" t="n">
+      <c r="AN13" t="n">
         <v>-0.5880635469517812</v>
       </c>
-      <c r="Z13" t="n">
+      <c r="AO13" t="n">
         <v>1.670062922416852</v>
       </c>
-      <c r="AA13" t="n">
+      <c r="AP13" t="n">
         <v>-0.3235545352841076</v>
       </c>
-      <c r="AB13" t="n">
+      <c r="AQ13" t="n">
         <v>1.929413722761977</v>
       </c>
-      <c r="AC13" t="n">
+      <c r="AR13" t="n">
         <v>-0.1912812391916924</v>
       </c>
-      <c r="AD13" t="n">
+      <c r="AS13" t="n">
         <v>2.032749027225145</v>
       </c>
-      <c r="AE13" t="n">
+      <c r="AT13" t="n">
         <v>-0.2528019830690212</v>
       </c>
-      <c r="AF13" t="n">
+      <c r="AU13" t="n">
         <v>-0.1122529741839473</v>
       </c>
-      <c r="AG13" t="n">
+      <c r="AV13" t="n">
         <v>-1.440633543338941</v>
       </c>
-      <c r="AH13" t="n">
+      <c r="AW13" t="n">
         <v>-0.8894682209233411</v>
       </c>
-      <c r="AI13" t="n">
+      <c r="AX13" t="n">
         <v>-1.011652984710315</v>
       </c>
-      <c r="AJ13" t="n">
+      <c r="AY13" t="n">
         <v>1.947692612537406</v>
       </c>
-      <c r="AK13" t="n">
+      <c r="AZ13" t="n">
         <v>0.9780422329392844</v>
       </c>
     </row>
@@ -1987,105 +2602,150 @@
         <v>2.75</v>
       </c>
       <c r="D14" t="n">
+        <v>256.3308827605442</v>
+      </c>
+      <c r="E14" t="n">
         <v>7.552788105416807</v>
       </c>
-      <c r="E14" t="n">
+      <c r="F14" t="n">
+        <v>243.9063500428031</v>
+      </c>
+      <c r="G14" t="n">
         <v>16.07013458901263</v>
       </c>
-      <c r="F14" t="n">
+      <c r="H14" t="n">
+        <v>228.5816431890988</v>
+      </c>
+      <c r="I14" t="n">
         <v>3.471439780918418</v>
       </c>
-      <c r="G14" t="n">
+      <c r="J14" t="n">
+        <v>227.8292437817188</v>
+      </c>
+      <c r="K14" t="n">
         <v>6.560652644921704</v>
       </c>
-      <c r="H14" t="n">
+      <c r="L14" t="n">
+        <v>224.0007829158864</v>
+      </c>
+      <c r="M14" t="n">
         <v>13.34916547680578</v>
       </c>
-      <c r="I14" t="n">
+      <c r="N14" t="n">
+        <v>231.3221655838879</v>
+      </c>
+      <c r="O14" t="n">
         <v>17.28631452465734</v>
       </c>
-      <c r="J14" t="n">
+      <c r="P14" t="n">
+        <v>228.0180679990891</v>
+      </c>
+      <c r="Q14" t="n">
         <v>24.95349315886802</v>
       </c>
-      <c r="K14" t="n">
+      <c r="R14" t="n">
+        <v>188.4268863826779</v>
+      </c>
+      <c r="S14" t="n">
         <v>26.8753134612496</v>
       </c>
-      <c r="L14" t="n">
+      <c r="T14" t="n">
+        <v>184.7464294298321</v>
+      </c>
+      <c r="U14" t="n">
         <v>18.4631293547069</v>
       </c>
-      <c r="M14" t="n">
+      <c r="V14" t="n">
+        <v>193.5260578250209</v>
+      </c>
+      <c r="W14" t="n">
         <v>14.10940555816001</v>
       </c>
-      <c r="N14" t="n">
+      <c r="X14" t="n">
+        <v>186.8440715979177</v>
+      </c>
+      <c r="Y14" t="n">
         <v>4.893695547225632</v>
       </c>
-      <c r="O14" t="n">
+      <c r="Z14" t="n">
+        <v>195.5585452681738</v>
+      </c>
+      <c r="AA14" t="n">
         <v>1.392692200681003</v>
       </c>
-      <c r="P14" t="n">
+      <c r="AB14" t="n">
+        <v>168.9428425849752</v>
+      </c>
+      <c r="AC14" t="n">
         <v>19.66274342638381</v>
       </c>
-      <c r="Q14" t="n">
+      <c r="AD14" t="n">
+        <v>136.4946314629088</v>
+      </c>
+      <c r="AE14" t="n">
         <v>33.86526750334612</v>
       </c>
-      <c r="R14" t="n">
+      <c r="AF14" t="n">
+        <v>103.705315471541</v>
+      </c>
+      <c r="AG14" t="n">
         <v>50.19970920914454</v>
       </c>
-      <c r="S14" t="n">
+      <c r="AH14" t="n">
         <v>75.57128208931118</v>
       </c>
-      <c r="T14" t="n">
+      <c r="AI14" t="n">
         <v>80.96523952800078</v>
       </c>
-      <c r="U14" t="n">
+      <c r="AJ14" t="n">
         <v>93.2217554444414</v>
       </c>
-      <c r="V14" t="n">
+      <c r="AK14" t="n">
         <v>0.3543608577538834</v>
       </c>
-      <c r="W14" t="n">
+      <c r="AL14" t="n">
         <v>-0.4138571362123425</v>
       </c>
-      <c r="X14" t="n">
+      <c r="AM14" t="n">
         <v>0.7221289983032428</v>
       </c>
-      <c r="Y14" t="n">
+      <c r="AN14" t="n">
         <v>-0.4415508280409143</v>
       </c>
-      <c r="Z14" t="n">
+      <c r="AO14" t="n">
         <v>1.466522402797187</v>
       </c>
-      <c r="AA14" t="n">
+      <c r="AP14" t="n">
         <v>-0.1786302167473129</v>
       </c>
-      <c r="AB14" t="n">
+      <c r="AQ14" t="n">
         <v>1.765863988416414</v>
       </c>
-      <c r="AC14" t="n">
+      <c r="AR14" t="n">
         <v>-0.07057471055510951</v>
       </c>
-      <c r="AD14" t="n">
+      <c r="AS14" t="n">
         <v>1.734357691825704</v>
       </c>
-      <c r="AE14" t="n">
+      <c r="AT14" t="n">
         <v>-0.1494349951439735</v>
       </c>
-      <c r="AF14" t="n">
+      <c r="AU14" t="n">
         <v>-1.611394138095491</v>
       </c>
-      <c r="AG14" t="n">
+      <c r="AV14" t="n">
         <v>-1.942223495686067</v>
       </c>
-      <c r="AH14" t="n">
+      <c r="AW14" t="n">
         <v>-2.205662430120638</v>
       </c>
-      <c r="AI14" t="n">
+      <c r="AX14" t="n">
         <v>-0.9104152910018912</v>
       </c>
-      <c r="AJ14" t="n">
+      <c r="AY14" t="n">
         <v>2.875930271682439</v>
       </c>
-      <c r="AK14" t="n">
+      <c r="AZ14" t="n">
         <v>1.257322200707738</v>
       </c>
     </row>
@@ -2100,105 +2760,150 @@
         <v>2.75</v>
       </c>
       <c r="D15" t="n">
+        <v>255.5381568611091</v>
+      </c>
+      <c r="E15" t="n">
         <v>6.552309347382672</v>
       </c>
-      <c r="E15" t="n">
+      <c r="F15" t="n">
+        <v>246.4718453427579</v>
+      </c>
+      <c r="G15" t="n">
         <v>15.91022843164755</v>
       </c>
-      <c r="F15" t="n">
+      <c r="H15" t="n">
+        <v>233.6152010775627</v>
+      </c>
+      <c r="I15" t="n">
         <v>3.936616072417995</v>
       </c>
-      <c r="G15" t="n">
+      <c r="J15" t="n">
+        <v>232.7943279388103</v>
+      </c>
+      <c r="K15" t="n">
         <v>6.501523146392607</v>
       </c>
-      <c r="H15" t="n">
+      <c r="L15" t="n">
+        <v>227.1594855802279</v>
+      </c>
+      <c r="M15" t="n">
         <v>13.62799313051481</v>
       </c>
-      <c r="I15" t="n">
+      <c r="N15" t="n">
+        <v>234.2907206809267</v>
+      </c>
+      <c r="O15" t="n">
         <v>17.48376941004543</v>
       </c>
-      <c r="J15" t="n">
+      <c r="P15" t="n">
+        <v>230.7135443315439</v>
+      </c>
+      <c r="Q15" t="n">
         <v>24.97681218681605</v>
       </c>
-      <c r="K15" t="n">
+      <c r="R15" t="n">
+        <v>190.281687222474</v>
+      </c>
+      <c r="S15" t="n">
         <v>26.60212584421145</v>
       </c>
-      <c r="L15" t="n">
+      <c r="T15" t="n">
+        <v>186.7721407971483</v>
+      </c>
+      <c r="U15" t="n">
         <v>18.243748414601</v>
       </c>
-      <c r="M15" t="n">
+      <c r="V15" t="n">
+        <v>195.0861110754893</v>
+      </c>
+      <c r="W15" t="n">
         <v>13.45027152528154</v>
       </c>
-      <c r="N15" t="n">
+      <c r="X15" t="n">
+        <v>187.3417035907718</v>
+      </c>
+      <c r="Y15" t="n">
         <v>5.031656035294767</v>
       </c>
-      <c r="O15" t="n">
+      <c r="Z15" t="n">
+        <v>195.7588787619949</v>
+      </c>
+      <c r="AA15" t="n">
         <v>1.021336156425746</v>
       </c>
-      <c r="P15" t="n">
+      <c r="AB15" t="n">
+        <v>171.4387707676448</v>
+      </c>
+      <c r="AC15" t="n">
         <v>19.60764979639798</v>
       </c>
-      <c r="Q15" t="n">
+      <c r="AD15" t="n">
+        <v>138.9515555919485</v>
+      </c>
+      <c r="AE15" t="n">
         <v>33.35982349747461</v>
       </c>
-      <c r="R15" t="n">
+      <c r="AF15" t="n">
+        <v>106.1272170104034</v>
+      </c>
+      <c r="AG15" t="n">
         <v>49.76446104387865</v>
       </c>
-      <c r="S15" t="n">
+      <c r="AH15" t="n">
         <v>72.16733180215698</v>
       </c>
-      <c r="T15" t="n">
+      <c r="AI15" t="n">
         <v>78.20740529773849</v>
       </c>
-      <c r="U15" t="n">
+      <c r="AJ15" t="n">
         <v>98.29193950852793</v>
       </c>
-      <c r="V15" t="n">
+      <c r="AK15" t="n">
         <v>0.07048278835648543</v>
       </c>
-      <c r="W15" t="n">
+      <c r="AL15" t="n">
         <v>-0.1877978127053436</v>
       </c>
-      <c r="X15" t="n">
+      <c r="AM15" t="n">
         <v>0.3620172646028805</v>
       </c>
-      <c r="Y15" t="n">
+      <c r="AN15" t="n">
         <v>-0.1991230756678468</v>
       </c>
-      <c r="Z15" t="n">
+      <c r="AO15" t="n">
         <v>1.318410398266841</v>
       </c>
-      <c r="AA15" t="n">
+      <c r="AP15" t="n">
         <v>-0.1888882183859544</v>
       </c>
-      <c r="AB15" t="n">
+      <c r="AQ15" t="n">
         <v>1.781259614525113</v>
       </c>
-      <c r="AC15" t="n">
+      <c r="AR15" t="n">
         <v>-0.08296336688048225</v>
       </c>
-      <c r="AD15" t="n">
+      <c r="AS15" t="n">
         <v>1.722845583097305</v>
       </c>
-      <c r="AE15" t="n">
+      <c r="AT15" t="n">
         <v>-0.003264981804164461</v>
       </c>
-      <c r="AF15" t="n">
+      <c r="AU15" t="n">
         <v>-3.471323631487306</v>
       </c>
-      <c r="AG15" t="n">
+      <c r="AV15" t="n">
         <v>-0.8564413191402948</v>
       </c>
-      <c r="AH15" t="n">
+      <c r="AW15" t="n">
         <v>-2.944951170158159</v>
       </c>
-      <c r="AI15" t="n">
+      <c r="AX15" t="n">
         <v>-0.2745222506882151</v>
       </c>
-      <c r="AJ15" t="n">
+      <c r="AY15" t="n">
         <v>4.145960878118291</v>
       </c>
-      <c r="AK15" t="n">
+      <c r="AZ15" t="n">
         <v>-0.03173091340426698</v>
       </c>
     </row>
@@ -2213,105 +2918,150 @@
         <v>2.75</v>
       </c>
       <c r="D16" t="n">
+        <v>240.0936363436652</v>
+      </c>
+      <c r="E16" t="n">
         <v>11.04275858994071</v>
       </c>
-      <c r="E16" t="n">
+      <c r="F16" t="n">
+        <v>248.8842470848814</v>
+      </c>
+      <c r="G16" t="n">
         <v>15.97096903104309</v>
       </c>
-      <c r="F16" t="n">
+      <c r="H16" t="n">
+        <v>240.5698758279179</v>
+      </c>
+      <c r="I16" t="n">
         <v>4.070464939090381</v>
       </c>
-      <c r="G16" t="n">
+      <c r="J16" t="n">
+        <v>238.7895442069845</v>
+      </c>
+      <c r="K16" t="n">
         <v>6.910427580488493</v>
       </c>
-      <c r="H16" t="n">
+      <c r="L16" t="n">
+        <v>230.5727240041638</v>
+      </c>
+      <c r="M16" t="n">
         <v>13.3239911803117</v>
       </c>
-      <c r="I16" t="n">
+      <c r="N16" t="n">
+        <v>237.1706069783962</v>
+      </c>
+      <c r="O16" t="n">
         <v>17.46298776450733</v>
       </c>
-      <c r="J16" t="n">
+      <c r="P16" t="n">
+        <v>233.7429021267181</v>
+      </c>
+      <c r="Q16" t="n">
         <v>24.80589684019697</v>
       </c>
-      <c r="K16" t="n">
+      <c r="R16" t="n">
+        <v>192.0757918493122</v>
+      </c>
+      <c r="S16" t="n">
         <v>26.12004246272094</v>
       </c>
-      <c r="L16" t="n">
+      <c r="T16" t="n">
+        <v>188.5258228220838</v>
+      </c>
+      <c r="U16" t="n">
         <v>17.76570157801851</v>
       </c>
-      <c r="M16" t="n">
+      <c r="V16" t="n">
+        <v>196.3989206239687</v>
+      </c>
+      <c r="W16" t="n">
         <v>12.50243220768922</v>
       </c>
-      <c r="N16" t="n">
+      <c r="X16" t="n">
+        <v>187.651647489967</v>
+      </c>
+      <c r="Y16" t="n">
         <v>5.234134619963087</v>
       </c>
-      <c r="O16" t="n">
+      <c r="Z16" t="n">
+        <v>195.7748110412706</v>
+      </c>
+      <c r="AA16" t="n">
         <v>0.6883502851986745</v>
       </c>
-      <c r="P16" t="n">
+      <c r="AB16" t="n">
+        <v>173.6024481184939</v>
+      </c>
+      <c r="AC16" t="n">
         <v>19.33048261818312</v>
       </c>
-      <c r="Q16" t="n">
+      <c r="AD16" t="n">
+        <v>141.2463730954109</v>
+      </c>
+      <c r="AE16" t="n">
         <v>32.9638531867494</v>
       </c>
-      <c r="R16" t="n">
+      <c r="AF16" t="n">
+        <v>108.5405638031926</v>
+      </c>
+      <c r="AG16" t="n">
         <v>49.03394381205241</v>
       </c>
-      <c r="S16" t="n">
+      <c r="AH16" t="n">
         <v>68.19132646369808</v>
       </c>
-      <c r="T16" t="n">
+      <c r="AI16" t="n">
         <v>74.23121782151131</v>
       </c>
-      <c r="U16" t="n">
+      <c r="AJ16" t="n">
         <v>101.5675575142986</v>
       </c>
-      <c r="V16" t="n">
+      <c r="AK16" t="n">
         <v>-0.00326434771220023</v>
       </c>
-      <c r="W16" t="n">
+      <c r="AL16" t="n">
         <v>-0.04793240668925933</v>
       </c>
-      <c r="X16" t="n">
+      <c r="AM16" t="n">
         <v>0.2809304717584697</v>
       </c>
-      <c r="Y16" t="n">
+      <c r="AN16" t="n">
         <v>-0.06896688583049551</v>
       </c>
-      <c r="Z16" t="n">
+      <c r="AO16" t="n">
         <v>1.074378456629759</v>
       </c>
-      <c r="AA16" t="n">
+      <c r="AP16" t="n">
         <v>-0.1124456419166944</v>
       </c>
-      <c r="AB16" t="n">
+      <c r="AQ16" t="n">
         <v>1.662895992292582</v>
       </c>
-      <c r="AC16" t="n">
+      <c r="AR16" t="n">
         <v>0.004530967550072845</v>
       </c>
-      <c r="AD16" t="n">
+      <c r="AS16" t="n">
         <v>1.841577739580306</v>
       </c>
-      <c r="AE16" t="n">
+      <c r="AT16" t="n">
         <v>0.07070573509162657</v>
       </c>
-      <c r="AF16" t="n">
+      <c r="AU16" t="n">
         <v>-3.391598028129684</v>
       </c>
-      <c r="AG16" t="n">
+      <c r="AV16" t="n">
         <v>0.02957534526604561</v>
       </c>
-      <c r="AH16" t="n">
+      <c r="AW16" t="n">
         <v>-2.435361249404284</v>
       </c>
-      <c r="AI16" t="n">
+      <c r="AX16" t="n">
         <v>0.4073673498420299</v>
       </c>
-      <c r="AJ16" t="n">
+      <c r="AY16" t="n">
         <v>2.928987832311851</v>
       </c>
-      <c r="AK16" t="n">
+      <c r="AZ16" t="n">
         <v>-0.04055315844870903</v>
       </c>
     </row>
@@ -2326,105 +3076,150 @@
         <v>2.75</v>
       </c>
       <c r="D17" t="n">
+        <v>259.579731597968</v>
+      </c>
+      <c r="E17" t="n">
         <v>9.297644162008943</v>
       </c>
-      <c r="E17" t="n">
+      <c r="F17" t="n">
+        <v>251.3708213436688</v>
+      </c>
+      <c r="G17" t="n">
         <v>16.23931810365501</v>
       </c>
-      <c r="F17" t="n">
+      <c r="H17" t="n">
+        <v>247.0949913593049</v>
+      </c>
+      <c r="I17" t="n">
         <v>4.708165310798804</v>
       </c>
-      <c r="G17" t="n">
+      <c r="J17" t="n">
+        <v>243.7163166331906</v>
+      </c>
+      <c r="K17" t="n">
         <v>6.970955463165927</v>
       </c>
-      <c r="H17" t="n">
+      <c r="L17" t="n">
+        <v>233.7039759818544</v>
+      </c>
+      <c r="M17" t="n">
         <v>12.67300632828517</v>
       </c>
-      <c r="I17" t="n">
+      <c r="N17" t="n">
+        <v>240.289472561356</v>
+      </c>
+      <c r="O17" t="n">
         <v>17.37718717426273</v>
       </c>
-      <c r="J17" t="n">
+      <c r="P17" t="n">
+        <v>236.3147713191121</v>
+      </c>
+      <c r="Q17" t="n">
         <v>24.85910780886386</v>
       </c>
-      <c r="K17" t="n">
+      <c r="R17" t="n">
+        <v>194.2132373228141</v>
+      </c>
+      <c r="S17" t="n">
         <v>25.95543759934446</v>
       </c>
-      <c r="L17" t="n">
+      <c r="T17" t="n">
+        <v>190.3889322957249</v>
+      </c>
+      <c r="U17" t="n">
         <v>17.70575097266664</v>
       </c>
-      <c r="M17" t="n">
+      <c r="V17" t="n">
+        <v>197.4200745846363</v>
+      </c>
+      <c r="W17" t="n">
         <v>11.97348621720118</v>
       </c>
-      <c r="N17" t="n">
+      <c r="X17" t="n">
+        <v>187.9552962932181</v>
+      </c>
+      <c r="Y17" t="n">
         <v>5.772179069248493</v>
       </c>
-      <c r="O17" t="n">
+      <c r="Z17" t="n">
+        <v>195.7207763448675</v>
+      </c>
+      <c r="AA17" t="n">
         <v>0.7860647025683225</v>
       </c>
-      <c r="P17" t="n">
+      <c r="AB17" t="n">
+        <v>175.8102460955897</v>
+      </c>
+      <c r="AC17" t="n">
         <v>19.28275054228221</v>
       </c>
-      <c r="Q17" t="n">
+      <c r="AD17" t="n">
+        <v>143.5939714418236</v>
+      </c>
+      <c r="AE17" t="n">
         <v>32.65134307509619</v>
       </c>
-      <c r="R17" t="n">
+      <c r="AF17" t="n">
+        <v>111.108708550744</v>
+      </c>
+      <c r="AG17" t="n">
         <v>48.79369397535392</v>
       </c>
-      <c r="S17" t="n">
+      <c r="AH17" t="n">
         <v>65.23551984873468</v>
       </c>
-      <c r="T17" t="n">
+      <c r="AI17" t="n">
         <v>73.00436847588057</v>
       </c>
-      <c r="U17" t="n">
+      <c r="AJ17" t="n">
         <v>105.0533357946617</v>
       </c>
-      <c r="V17" t="n">
+      <c r="AK17" t="n">
         <v>-0.03587117431856898</v>
       </c>
-      <c r="W17" t="n">
+      <c r="AL17" t="n">
         <v>0.01940693415648886</v>
       </c>
-      <c r="X17" t="n">
+      <c r="AM17" t="n">
         <v>0.2086025180546091</v>
       </c>
-      <c r="Y17" t="n">
+      <c r="AN17" t="n">
         <v>0.01833692510077452</v>
       </c>
-      <c r="Z17" t="n">
+      <c r="AO17" t="n">
         <v>1.095623031575628</v>
       </c>
-      <c r="AA17" t="n">
+      <c r="AP17" t="n">
         <v>0.07492248893629716</v>
       </c>
-      <c r="AB17" t="n">
+      <c r="AQ17" t="n">
         <v>1.79337660471598</v>
       </c>
-      <c r="AC17" t="n">
+      <c r="AR17" t="n">
         <v>0.103884364696258</v>
       </c>
-      <c r="AD17" t="n">
+      <c r="AS17" t="n">
         <v>1.841546922710772</v>
       </c>
-      <c r="AE17" t="n">
+      <c r="AT17" t="n">
         <v>0.01132932115108085</v>
       </c>
-      <c r="AF17" t="n">
+      <c r="AU17" t="n">
         <v>-3.486450813081813</v>
       </c>
-      <c r="AG17" t="n">
+      <c r="AV17" t="n">
         <v>-0.07899815436926168</v>
       </c>
-      <c r="AH17" t="n">
+      <c r="AW17" t="n">
         <v>-2.323964205559033</v>
       </c>
-      <c r="AI17" t="n">
+      <c r="AX17" t="n">
         <v>0.00595605839020194</v>
       </c>
-      <c r="AJ17" t="n">
+      <c r="AY17" t="n">
         <v>4.284958785317244</v>
       </c>
-      <c r="AK17" t="n">
+      <c r="AZ17" t="n">
         <v>0.9447311500939517</v>
       </c>
     </row>
@@ -2439,105 +3234,150 @@
         <v>2.75</v>
       </c>
       <c r="D18" t="n">
+        <v>237.9594345544036</v>
+      </c>
+      <c r="E18" t="n">
         <v>8.715788861538503</v>
       </c>
-      <c r="E18" t="n">
+      <c r="F18" t="n">
+        <v>253.6428764092584</v>
+      </c>
+      <c r="G18" t="n">
         <v>16.31835234080646</v>
       </c>
-      <c r="F18" t="n">
+      <c r="H18" t="n">
+        <v>251.1772124796894</v>
+      </c>
+      <c r="I18" t="n">
         <v>4.459999300909381</v>
       </c>
-      <c r="G18" t="n">
+      <c r="J18" t="n">
+        <v>247.478201076494</v>
+      </c>
+      <c r="K18" t="n">
         <v>6.279856093386388</v>
       </c>
-      <c r="H18" t="n">
+      <c r="L18" t="n">
+        <v>236.9382616475964</v>
+      </c>
+      <c r="M18" t="n">
         <v>11.96323049829361</v>
       </c>
-      <c r="I18" t="n">
+      <c r="N18" t="n">
+        <v>243.2540350349237</v>
+      </c>
+      <c r="O18" t="n">
         <v>16.92145428758986</v>
       </c>
-      <c r="J18" t="n">
+      <c r="P18" t="n">
+        <v>239.4326687704587</v>
+      </c>
+      <c r="Q18" t="n">
         <v>24.55830404944454</v>
       </c>
-      <c r="K18" t="n">
+      <c r="R18" t="n">
+        <v>196.2908776939338</v>
+      </c>
+      <c r="S18" t="n">
         <v>25.64929410920921</v>
       </c>
-      <c r="L18" t="n">
+      <c r="T18" t="n">
+        <v>192.591532578705</v>
+      </c>
+      <c r="U18" t="n">
         <v>17.39048518187611</v>
       </c>
-      <c r="M18" t="n">
+      <c r="V18" t="n">
+        <v>198.9052698121849</v>
+      </c>
+      <c r="W18" t="n">
         <v>11.2569250959031</v>
       </c>
-      <c r="N18" t="n">
+      <c r="X18" t="n">
+        <v>188.1673478065653</v>
+      </c>
+      <c r="Y18" t="n">
         <v>6.305336444935896</v>
       </c>
-      <c r="O18" t="n">
+      <c r="Z18" t="n">
+        <v>195.6520491458</v>
+      </c>
+      <c r="AA18" t="n">
         <v>0.7536066339371016</v>
       </c>
-      <c r="P18" t="n">
+      <c r="AB18" t="n">
+        <v>178.13262212361</v>
+      </c>
+      <c r="AC18" t="n">
         <v>19.06439970571099</v>
       </c>
-      <c r="Q18" t="n">
+      <c r="AD18" t="n">
+        <v>146.1272445976311</v>
+      </c>
+      <c r="AE18" t="n">
         <v>32.27462853100283</v>
       </c>
-      <c r="R18" t="n">
+      <c r="AF18" t="n">
+        <v>113.635079615505</v>
+      </c>
+      <c r="AG18" t="n">
         <v>48.50852709289984</v>
       </c>
-      <c r="S18" t="n">
+      <c r="AH18" t="n">
         <v>60.66038933251562</v>
       </c>
-      <c r="T18" t="n">
+      <c r="AI18" t="n">
         <v>69.40205911023693</v>
       </c>
-      <c r="U18" t="n">
+      <c r="AJ18" t="n">
         <v>110.7750975454493</v>
       </c>
-      <c r="V18" t="n">
+      <c r="AK18" t="n">
         <v>-0.00080804452828135</v>
       </c>
-      <c r="W18" t="n">
+      <c r="AL18" t="n">
         <v>0.01834607716147674</v>
       </c>
-      <c r="X18" t="n">
+      <c r="AM18" t="n">
         <v>0.2918675436195776</v>
       </c>
-      <c r="Y18" t="n">
+      <c r="AN18" t="n">
         <v>0.08224335545343514</v>
       </c>
-      <c r="Z18" t="n">
+      <c r="AO18" t="n">
         <v>1.135959354698241</v>
       </c>
-      <c r="AA18" t="n">
+      <c r="AP18" t="n">
         <v>-0.1219257606682217</v>
       </c>
-      <c r="AB18" t="n">
+      <c r="AQ18" t="n">
         <v>1.888317842010067</v>
       </c>
-      <c r="AC18" t="n">
+      <c r="AR18" t="n">
         <v>-0.05970939676812181</v>
       </c>
-      <c r="AD18" t="n">
+      <c r="AS18" t="n">
         <v>1.893801553874995</v>
       </c>
-      <c r="AE18" t="n">
+      <c r="AT18" t="n">
         <v>0.02524068592287923</v>
       </c>
-      <c r="AF18" t="n">
+      <c r="AU18" t="n">
         <v>-3.335457869055253</v>
       </c>
-      <c r="AG18" t="n">
+      <c r="AV18" t="n">
         <v>1.000015366706184</v>
       </c>
-      <c r="AH18" t="n">
+      <c r="AW18" t="n">
         <v>-1.888960110836099</v>
       </c>
-      <c r="AI18" t="n">
+      <c r="AX18" t="n">
         <v>0.9074936307799593</v>
       </c>
-      <c r="AJ18" t="n">
+      <c r="AY18" t="n">
         <v>5.26278118476765</v>
       </c>
-      <c r="AK18" t="n">
+      <c r="AZ18" t="n">
         <v>0.2496429322442716</v>
       </c>
     </row>
@@ -2552,105 +3392,150 @@
         <v>2.75</v>
       </c>
       <c r="D19" t="n">
+        <v>231.4730253823577</v>
+      </c>
+      <c r="E19" t="n">
         <v>9.101466929658928</v>
       </c>
-      <c r="E19" t="n">
+      <c r="F19" t="n">
+        <v>255.6208324770556</v>
+      </c>
+      <c r="G19" t="n">
         <v>16.18260559460795</v>
       </c>
-      <c r="F19" t="n">
+      <c r="H19" t="n">
+        <v>254.2082214186378</v>
+      </c>
+      <c r="I19" t="n">
         <v>4.293654827361406</v>
       </c>
-      <c r="G19" t="n">
+      <c r="J19" t="n">
+        <v>250.2383987531595</v>
+      </c>
+      <c r="K19" t="n">
         <v>5.895733326039411</v>
       </c>
-      <c r="H19" t="n">
+      <c r="L19" t="n">
+        <v>239.9828073826242</v>
+      </c>
+      <c r="M19" t="n">
         <v>11.63360615994068</v>
       </c>
-      <c r="I19" t="n">
+      <c r="N19" t="n">
+        <v>246.0701981757549</v>
+      </c>
+      <c r="O19" t="n">
         <v>16.63649166729433</v>
       </c>
-      <c r="J19" t="n">
+      <c r="P19" t="n">
+        <v>242.1635644232974</v>
+      </c>
+      <c r="Q19" t="n">
         <v>24.29021131907794</v>
       </c>
-      <c r="K19" t="n">
+      <c r="R19" t="n">
+        <v>198.5278697724038</v>
+      </c>
+      <c r="S19" t="n">
         <v>25.54332584354049</v>
       </c>
-      <c r="L19" t="n">
+      <c r="T19" t="n">
+        <v>194.5433711329251</v>
+      </c>
+      <c r="U19" t="n">
         <v>17.28267230040639</v>
       </c>
-      <c r="M19" t="n">
+      <c r="V19" t="n">
+        <v>199.856562479168</v>
+      </c>
+      <c r="W19" t="n">
         <v>10.41394734213538</v>
       </c>
-      <c r="N19" t="n">
+      <c r="X19" t="n">
+        <v>188.4878210987605</v>
+      </c>
+      <c r="Y19" t="n">
         <v>7.141250245114588</v>
       </c>
-      <c r="O19" t="n">
+      <c r="Z19" t="n">
+        <v>195.7235684631564</v>
+      </c>
+      <c r="AA19" t="n">
         <v>0.7023023375382649</v>
       </c>
-      <c r="P19" t="n">
+      <c r="AB19" t="n">
+        <v>180.5674290826135</v>
+      </c>
+      <c r="AC19" t="n">
         <v>18.8978540136459</v>
       </c>
-      <c r="Q19" t="n">
+      <c r="AD19" t="n">
+        <v>148.8173286965553</v>
+      </c>
+      <c r="AE19" t="n">
         <v>31.8598617053201</v>
       </c>
-      <c r="R19" t="n">
+      <c r="AF19" t="n">
+        <v>116.5464560190837</v>
+      </c>
+      <c r="AG19" t="n">
         <v>48.11760855059253</v>
       </c>
-      <c r="S19" t="n">
+      <c r="AH19" t="n">
         <v>57.7283445467028</v>
       </c>
-      <c r="T19" t="n">
+      <c r="AI19" t="n">
         <v>68.66982026790353</v>
       </c>
-      <c r="U19" t="n">
+      <c r="AJ19" t="n">
         <v>116.759154358329</v>
       </c>
-      <c r="V19" t="n">
+      <c r="AK19" t="n">
         <v>-0.006574561409919823</v>
       </c>
-      <c r="W19" t="n">
+      <c r="AL19" t="n">
         <v>-0.08974102794701733</v>
       </c>
-      <c r="X19" t="n">
+      <c r="AM19" t="n">
         <v>0.37650571647265</v>
       </c>
-      <c r="Y19" t="n">
+      <c r="AN19" t="n">
         <v>0.1804739659559641</v>
       </c>
-      <c r="Z19" t="n">
+      <c r="AO19" t="n">
         <v>1.006608651884899</v>
       </c>
-      <c r="AA19" t="n">
+      <c r="AP19" t="n">
         <v>0.03444869467552389</v>
       </c>
-      <c r="AB19" t="n">
+      <c r="AQ19" t="n">
         <v>1.743772351149973</v>
       </c>
-      <c r="AC19" t="n">
+      <c r="AR19" t="n">
         <v>0.03009780924371024</v>
       </c>
-      <c r="AD19" t="n">
+      <c r="AS19" t="n">
         <v>2.001566667083309</v>
       </c>
-      <c r="AE19" t="n">
+      <c r="AT19" t="n">
         <v>0.0552837307571544</v>
       </c>
-      <c r="AF19" t="n">
+      <c r="AU19" t="n">
         <v>-2.024297238229579</v>
       </c>
-      <c r="AG19" t="n">
+      <c r="AV19" t="n">
         <v>1.485307650602326</v>
       </c>
-      <c r="AH19" t="n">
+      <c r="AW19" t="n">
         <v>-1.418512914545619</v>
       </c>
-      <c r="AI19" t="n">
+      <c r="AX19" t="n">
         <v>0.5117275856149124</v>
       </c>
-      <c r="AJ19" t="n">
+      <c r="AY19" t="n">
         <v>4.486568314846595</v>
       </c>
-      <c r="AK19" t="n">
+      <c r="AZ19" t="n">
         <v>-0.04277589832961479</v>
       </c>
     </row>
@@ -2665,105 +3550,150 @@
         <v>2.75</v>
       </c>
       <c r="D20" t="n">
+        <v>233.2041191624094</v>
+      </c>
+      <c r="E20" t="n">
         <v>9.354179801670369</v>
       </c>
-      <c r="E20" t="n">
+      <c r="F20" t="n">
+        <v>257.3390416431089</v>
+      </c>
+      <c r="G20" t="n">
         <v>16.50955423395685</v>
       </c>
-      <c r="F20" t="n">
+      <c r="H20" t="n">
+        <v>256.9239668389584</v>
+      </c>
+      <c r="I20" t="n">
         <v>6.01773228205688</v>
       </c>
-      <c r="G20" t="n">
+      <c r="J20" t="n">
+        <v>252.8682810617677</v>
+      </c>
+      <c r="K20" t="n">
         <v>5.774016414128296</v>
       </c>
-      <c r="H20" t="n">
+      <c r="L20" t="n">
+        <v>242.9100046343837</v>
+      </c>
+      <c r="M20" t="n">
         <v>11.57948345157271</v>
       </c>
-      <c r="I20" t="n">
+      <c r="N20" t="n">
+        <v>248.6158147137216</v>
+      </c>
+      <c r="O20" t="n">
         <v>16.6382630666097</v>
       </c>
-      <c r="J20" t="n">
+      <c r="P20" t="n">
+        <v>244.7161298271612</v>
+      </c>
+      <c r="Q20" t="n">
         <v>24.35487043773029</v>
       </c>
-      <c r="K20" t="n">
+      <c r="R20" t="n">
+        <v>200.6453380517081</v>
+      </c>
+      <c r="S20" t="n">
         <v>25.36054130987073</v>
       </c>
-      <c r="L20" t="n">
+      <c r="T20" t="n">
+        <v>196.5247932055318</v>
+      </c>
+      <c r="U20" t="n">
         <v>17.22569939092541</v>
       </c>
-      <c r="M20" t="n">
+      <c r="V20" t="n">
+        <v>201.1065166892735</v>
+      </c>
+      <c r="W20" t="n">
         <v>9.797372547447251</v>
       </c>
-      <c r="N20" t="n">
+      <c r="X20" t="n">
+        <v>188.9201791573924</v>
+      </c>
+      <c r="Y20" t="n">
         <v>8.160734514818119</v>
       </c>
-      <c r="O20" t="n">
+      <c r="Z20" t="n">
+        <v>195.5625624521404</v>
+      </c>
+      <c r="AA20" t="n">
         <v>0.616609289291051</v>
       </c>
-      <c r="P20" t="n">
+      <c r="AB20" t="n">
+        <v>182.9820904325932</v>
+      </c>
+      <c r="AC20" t="n">
         <v>18.64015126059241</v>
       </c>
-      <c r="Q20" t="n">
+      <c r="AD20" t="n">
+        <v>151.6342309349818</v>
+      </c>
+      <c r="AE20" t="n">
         <v>31.41739977167008</v>
       </c>
-      <c r="R20" t="n">
+      <c r="AF20" t="n">
+        <v>120.1559642527966</v>
+      </c>
+      <c r="AG20" t="n">
         <v>47.16004987135001</v>
       </c>
-      <c r="S20" t="n">
+      <c r="AH20" t="n">
         <v>56.18890283263198</v>
       </c>
-      <c r="T20" t="n">
+      <c r="AI20" t="n">
         <v>66.09068538529294</v>
       </c>
-      <c r="U20" t="n">
+      <c r="AJ20" t="n">
         <v>121.9105157568757</v>
       </c>
-      <c r="V20" t="n">
+      <c r="AK20" t="n">
         <v>-0.1331588055225134</v>
       </c>
-      <c r="W20" t="n">
+      <c r="AL20" t="n">
         <v>-0.04208772740465376</v>
       </c>
-      <c r="X20" t="n">
+      <c r="AM20" t="n">
         <v>0.6491745194644786</v>
       </c>
-      <c r="Y20" t="n">
+      <c r="AN20" t="n">
         <v>0.2864004026913491</v>
       </c>
-      <c r="Z20" t="n">
+      <c r="AO20" t="n">
         <v>1.046691634130814</v>
       </c>
-      <c r="AA20" t="n">
+      <c r="AP20" t="n">
         <v>-0.02743766662921991</v>
       </c>
-      <c r="AB20" t="n">
+      <c r="AQ20" t="n">
         <v>1.923721479185928</v>
       </c>
-      <c r="AC20" t="n">
+      <c r="AR20" t="n">
         <v>0.1194979070771642</v>
       </c>
-      <c r="AD20" t="n">
+      <c r="AS20" t="n">
         <v>1.953367984041256</v>
       </c>
-      <c r="AE20" t="n">
+      <c r="AT20" t="n">
         <v>0.0943715267992995</v>
       </c>
-      <c r="AF20" t="n">
+      <c r="AU20" t="n">
         <v>-0.3108039559925441</v>
       </c>
-      <c r="AG20" t="n">
+      <c r="AV20" t="n">
         <v>1.911259692257916</v>
       </c>
-      <c r="AH20" t="n">
+      <c r="AW20" t="n">
         <v>0.06482757201835082</v>
       </c>
-      <c r="AI20" t="n">
+      <c r="AX20" t="n">
         <v>1.580430699153635</v>
       </c>
-      <c r="AJ20" t="n">
+      <c r="AY20" t="n">
         <v>6.057442209654397</v>
       </c>
-      <c r="AK20" t="n">
+      <c r="AZ20" t="n">
         <v>0.7895700299442874</v>
       </c>
     </row>
@@ -2778,105 +3708,150 @@
         <v>2.75</v>
       </c>
       <c r="D21" t="n">
+        <v>246.7908776873815</v>
+      </c>
+      <c r="E21" t="n">
         <v>8.736013520693945</v>
       </c>
-      <c r="E21" t="n">
+      <c r="F21" t="n">
+        <v>254.3112276716436</v>
+      </c>
+      <c r="G21" t="n">
         <v>17.23814754621356</v>
       </c>
-      <c r="F21" t="n">
+      <c r="H21" t="n">
+        <v>254.2140755987336</v>
+      </c>
+      <c r="I21" t="n">
         <v>3.873880873335167</v>
       </c>
-      <c r="G21" t="n">
+      <c r="J21" t="n">
+        <v>255.5505946595618</v>
+      </c>
+      <c r="K21" t="n">
         <v>5.484145752927088</v>
       </c>
-      <c r="H21" t="n">
+      <c r="L21" t="n">
+        <v>245.8245507791533</v>
+      </c>
+      <c r="M21" t="n">
         <v>11.53016191847781</v>
       </c>
-      <c r="I21" t="n">
+      <c r="N21" t="n">
+        <v>251.3361525451038</v>
+      </c>
+      <c r="O21" t="n">
         <v>16.66860918626717</v>
       </c>
-      <c r="J21" t="n">
+      <c r="P21" t="n">
+        <v>247.2681546676243</v>
+      </c>
+      <c r="Q21" t="n">
         <v>24.37902105615494</v>
       </c>
-      <c r="K21" t="n">
+      <c r="R21" t="n">
+        <v>203.1381860692451</v>
+      </c>
+      <c r="S21" t="n">
         <v>25.47215130312223</v>
       </c>
-      <c r="L21" t="n">
+      <c r="T21" t="n">
+        <v>198.84769713625</v>
+      </c>
+      <c r="U21" t="n">
         <v>17.40496479873116</v>
       </c>
-      <c r="M21" t="n">
+      <c r="V21" t="n">
+        <v>202.246094595456</v>
+      </c>
+      <c r="W21" t="n">
         <v>9.216811132769207</v>
       </c>
-      <c r="N21" t="n">
+      <c r="X21" t="n">
+        <v>189.7603392601013</v>
+      </c>
+      <c r="Y21" t="n">
         <v>9.094153059289813</v>
       </c>
-      <c r="O21" t="n">
+      <c r="Z21" t="n">
+        <v>195.423535421385</v>
+      </c>
+      <c r="AA21" t="n">
         <v>0.7082830929587078</v>
       </c>
-      <c r="P21" t="n">
+      <c r="AB21" t="n">
+        <v>185.4167441104321</v>
+      </c>
+      <c r="AC21" t="n">
         <v>18.78505057476937</v>
       </c>
-      <c r="Q21" t="n">
+      <c r="AD21" t="n">
+        <v>154.5323978079126</v>
+      </c>
+      <c r="AE21" t="n">
         <v>31.14451651877546</v>
       </c>
-      <c r="R21" t="n">
+      <c r="AF21" t="n">
+        <v>123.5217880695424</v>
+      </c>
+      <c r="AG21" t="n">
         <v>46.41669912541167</v>
       </c>
-      <c r="S21" t="n">
+      <c r="AH21" t="n">
         <v>56.25536334024934</v>
       </c>
-      <c r="T21" t="n">
+      <c r="AI21" t="n">
         <v>67.76304780275403</v>
       </c>
-      <c r="U21" t="n">
+      <c r="AJ21" t="n">
         <v>129.3921759181256</v>
       </c>
-      <c r="V21" t="n">
+      <c r="AK21" t="n">
         <v>-0.1327667253237254</v>
       </c>
-      <c r="W21" t="n">
+      <c r="AL21" t="n">
         <v>0.03836049255749996</v>
       </c>
-      <c r="X21" t="n">
+      <c r="AM21" t="n">
         <v>1.011429779918483</v>
       </c>
-      <c r="Y21" t="n">
+      <c r="AN21" t="n">
         <v>0.2374146635650732</v>
       </c>
-      <c r="Z21" t="n">
+      <c r="AO21" t="n">
         <v>1.075426652921855</v>
       </c>
-      <c r="AA21" t="n">
+      <c r="AP21" t="n">
         <v>0.07043108872487981</v>
       </c>
-      <c r="AB21" t="n">
+      <c r="AQ21" t="n">
         <v>1.945644617080689</v>
       </c>
-      <c r="AC21" t="n">
+      <c r="AR21" t="n">
         <v>0.03508735210338002</v>
       </c>
-      <c r="AD21" t="n">
+      <c r="AS21" t="n">
         <v>2.187192270941766</v>
       </c>
-      <c r="AE21" t="n">
+      <c r="AT21" t="n">
         <v>0.023619545266986</v>
       </c>
-      <c r="AF21" t="n">
+      <c r="AU21" t="n">
         <v>2.158570469093129</v>
       </c>
-      <c r="AG21" t="n">
+      <c r="AV21" t="n">
         <v>1.655275446745006</v>
       </c>
-      <c r="AH21" t="n">
+      <c r="AW21" t="n">
         <v>1.257059315083873</v>
       </c>
-      <c r="AI21" t="n">
+      <c r="AX21" t="n">
         <v>0.756052196953014</v>
       </c>
-      <c r="AJ21" t="n">
+      <c r="AY21" t="n">
         <v>4.948269926704763</v>
       </c>
-      <c r="AK21" t="n">
+      <c r="AZ21" t="n">
         <v>-0.2123678536455198</v>
       </c>
     </row>
@@ -2891,105 +3866,150 @@
         <v>2.75</v>
       </c>
       <c r="D22" t="n">
+        <v>221.7479559295672</v>
+      </c>
+      <c r="E22" t="n">
         <v>14.04394393271589</v>
       </c>
-      <c r="E22" t="n">
+      <c r="F22" t="n">
+        <v>256.2191195574635</v>
+      </c>
+      <c r="G22" t="n">
         <v>17.91878355310318</v>
       </c>
-      <c r="F22" t="n">
+      <c r="H22" t="n">
+        <v>255.5657514707839</v>
+      </c>
+      <c r="I22" t="n">
         <v>3.195735241504425</v>
       </c>
-      <c r="G22" t="n">
+      <c r="J22" t="n">
+        <v>257.0068494647953</v>
+      </c>
+      <c r="K22" t="n">
         <v>5.003057304003557</v>
       </c>
-      <c r="H22" t="n">
+      <c r="L22" t="n">
+        <v>248.3313645031436</v>
+      </c>
+      <c r="M22" t="n">
         <v>11.34717785720284</v>
       </c>
-      <c r="I22" t="n">
+      <c r="N22" t="n">
+        <v>253.8477803005817</v>
+      </c>
+      <c r="O22" t="n">
         <v>16.69436008372205</v>
       </c>
-      <c r="J22" t="n">
+      <c r="P22" t="n">
+        <v>250.0689800960798</v>
+      </c>
+      <c r="Q22" t="n">
         <v>24.44053338774552</v>
       </c>
-      <c r="K22" t="n">
+      <c r="R22" t="n">
+        <v>205.3594568942456</v>
+      </c>
+      <c r="S22" t="n">
         <v>25.53797224734692</v>
       </c>
-      <c r="L22" t="n">
+      <c r="T22" t="n">
+        <v>200.9787949264472</v>
+      </c>
+      <c r="U22" t="n">
         <v>17.49113299322467</v>
       </c>
-      <c r="M22" t="n">
+      <c r="V22" t="n">
+        <v>203.4262910802314</v>
+      </c>
+      <c r="W22" t="n">
         <v>8.87680256620367</v>
       </c>
-      <c r="N22" t="n">
+      <c r="X22" t="n">
+        <v>191.0654118720522</v>
+      </c>
+      <c r="Y22" t="n">
         <v>9.776867196914999</v>
       </c>
-      <c r="O22" t="n">
+      <c r="Z22" t="n">
+        <v>195.2689235092055</v>
+      </c>
+      <c r="AA22" t="n">
         <v>0.8535270149826145</v>
       </c>
-      <c r="P22" t="n">
+      <c r="AB22" t="n">
+        <v>187.903587699782</v>
+      </c>
+      <c r="AC22" t="n">
         <v>18.98585346573634</v>
       </c>
-      <c r="Q22" t="n">
+      <c r="AD22" t="n">
+        <v>157.1327299936443</v>
+      </c>
+      <c r="AE22" t="n">
         <v>31.39917816676147</v>
       </c>
-      <c r="R22" t="n">
+      <c r="AF22" t="n">
+        <v>126.3210561258573</v>
+      </c>
+      <c r="AG22" t="n">
         <v>46.35519423383349</v>
       </c>
-      <c r="S22" t="n">
+      <c r="AH22" t="n">
         <v>60.04168933112581</v>
       </c>
-      <c r="T22" t="n">
+      <c r="AI22" t="n">
         <v>69.84654160980274</v>
       </c>
-      <c r="U22" t="n">
+      <c r="AJ22" t="n">
         <v>135.7135812559167</v>
       </c>
-      <c r="V22" t="n">
+      <c r="AK22" t="n">
         <v>-0.04174058318983513</v>
       </c>
-      <c r="W22" t="n">
+      <c r="AL22" t="n">
         <v>0.09020607099465465</v>
       </c>
-      <c r="X22" t="n">
+      <c r="AM22" t="n">
         <v>1.136916749020837</v>
       </c>
-      <c r="Y22" t="n">
+      <c r="AN22" t="n">
         <v>0.164829923751505</v>
       </c>
-      <c r="Z22" t="n">
+      <c r="AO22" t="n">
         <v>1.122568008747502</v>
       </c>
-      <c r="AA22" t="n">
+      <c r="AP22" t="n">
         <v>0.1094242782457485</v>
       </c>
-      <c r="AB22" t="n">
+      <c r="AQ22" t="n">
         <v>2.048225690287058</v>
       </c>
-      <c r="AC22" t="n">
+      <c r="AR22" t="n">
         <v>0.09876413548246177</v>
       </c>
-      <c r="AD22" t="n">
+      <c r="AS22" t="n">
         <v>1.997011012219367</v>
       </c>
-      <c r="AE22" t="n">
+      <c r="AT22" t="n">
         <v>0.08040383352455227</v>
       </c>
-      <c r="AF22" t="n">
+      <c r="AU22" t="n">
         <v>3.176558634842332</v>
       </c>
-      <c r="AG22" t="n">
+      <c r="AV22" t="n">
         <v>0.9648395539426673</v>
       </c>
-      <c r="AH22" t="n">
+      <c r="AW22" t="n">
         <v>2.040719043502751</v>
       </c>
-      <c r="AI22" t="n">
+      <c r="AX22" t="n">
         <v>0.2573631113211186</v>
       </c>
-      <c r="AJ22" t="n">
+      <c r="AY22" t="n">
         <v>6.426433412010974</v>
       </c>
-      <c r="AK22" t="n">
+      <c r="AZ22" t="n">
         <v>-0.3241097889575698</v>
       </c>
     </row>
@@ -3004,105 +4024,150 @@
         <v>2.75</v>
       </c>
       <c r="D23" t="n">
+        <v>226.2159490825754</v>
+      </c>
+      <c r="E23" t="n">
         <v>15.76714312776606</v>
       </c>
-      <c r="E23" t="n">
+      <c r="F23" t="n">
+        <v>258.0374934677537</v>
+      </c>
+      <c r="G23" t="n">
         <v>18.78787980857471</v>
       </c>
-      <c r="F23" t="n">
+      <c r="H23" t="n">
+        <v>256.4181626899868</v>
+      </c>
+      <c r="I23" t="n">
         <v>2.785203811970166</v>
       </c>
-      <c r="G23" t="n">
+      <c r="J23" t="n">
+        <v>257.9838913383214</v>
+      </c>
+      <c r="K23" t="n">
         <v>4.666519841403826</v>
       </c>
-      <c r="H23" t="n">
+      <c r="L23" t="n">
+        <v>250.4643924270116</v>
+      </c>
+      <c r="M23" t="n">
         <v>11.53864860534668</v>
       </c>
-      <c r="I23" t="n">
+      <c r="N23" t="n">
+        <v>255.8677494763694</v>
+      </c>
+      <c r="O23" t="n">
         <v>16.84157391811939</v>
       </c>
-      <c r="J23" t="n">
+      <c r="P23" t="n">
+        <v>251.6295992102184</v>
+      </c>
+      <c r="Q23" t="n">
         <v>24.86710582219118</v>
       </c>
-      <c r="K23" t="n">
+      <c r="R23" t="n">
+        <v>207.7984464929459</v>
+      </c>
+      <c r="S23" t="n">
         <v>25.41782044349833</v>
       </c>
-      <c r="L23" t="n">
+      <c r="T23" t="n">
+        <v>203.3694020399811</v>
+      </c>
+      <c r="U23" t="n">
         <v>17.41398412285122</v>
       </c>
-      <c r="M23" t="n">
+      <c r="V23" t="n">
+        <v>204.7019236476709</v>
+      </c>
+      <c r="W23" t="n">
         <v>8.437672067195813</v>
       </c>
-      <c r="N23" t="n">
+      <c r="X23" t="n">
+        <v>192.3294516319924</v>
+      </c>
+      <c r="Y23" t="n">
         <v>10.42824400232193</v>
       </c>
-      <c r="O23" t="n">
+      <c r="Z23" t="n">
+        <v>195.2791854844871</v>
+      </c>
+      <c r="AA23" t="n">
         <v>0.8193817544490675</v>
       </c>
-      <c r="P23" t="n">
+      <c r="AB23" t="n">
+        <v>190.3760754470284</v>
+      </c>
+      <c r="AC23" t="n">
         <v>19.0207376547739</v>
       </c>
-      <c r="Q23" t="n">
+      <c r="AD23" t="n">
+        <v>159.8998978628335</v>
+      </c>
+      <c r="AE23" t="n">
         <v>31.74785705322914</v>
       </c>
-      <c r="R23" t="n">
+      <c r="AF23" t="n">
+        <v>129.0594335988904</v>
+      </c>
+      <c r="AG23" t="n">
         <v>46.87951186024551</v>
       </c>
-      <c r="S23" t="n">
+      <c r="AH23" t="n">
         <v>63.39240033790633</v>
       </c>
-      <c r="T23" t="n">
+      <c r="AI23" t="n">
         <v>72.45447395430811</v>
       </c>
-      <c r="U23" t="n">
+      <c r="AJ23" t="n">
         <v>142.7276586482517</v>
       </c>
-      <c r="V23" t="n">
+      <c r="AK23" t="n">
         <v>0.0501977636459036</v>
       </c>
-      <c r="W23" t="n">
+      <c r="AL23" t="n">
         <v>0.1068015259208416</v>
       </c>
-      <c r="X23" t="n">
+      <c r="AM23" t="n">
         <v>1.376119150337596</v>
       </c>
-      <c r="Y23" t="n">
+      <c r="AN23" t="n">
         <v>0.2676227836744197</v>
       </c>
-      <c r="Z23" t="n">
+      <c r="AO23" t="n">
         <v>1.27354775760191</v>
       </c>
-      <c r="AA23" t="n">
+      <c r="AP23" t="n">
         <v>0.1960421284885316</v>
       </c>
-      <c r="AB23" t="n">
+      <c r="AQ23" t="n">
         <v>2.118711141829796</v>
       </c>
-      <c r="AC23" t="n">
+      <c r="AR23" t="n">
         <v>0.007781703421408267</v>
       </c>
-      <c r="AD23" t="n">
+      <c r="AS23" t="n">
         <v>2.323626457376683</v>
       </c>
-      <c r="AE23" t="n">
+      <c r="AT23" t="n">
         <v>0.1083901587953001</v>
       </c>
-      <c r="AF23" t="n">
+      <c r="AU23" t="n">
         <v>4.433834007388858</v>
       </c>
-      <c r="AG23" t="n">
+      <c r="AV23" t="n">
         <v>1.357375421155441</v>
       </c>
-      <c r="AH23" t="n">
+      <c r="AW23" t="n">
         <v>2.332030595382983</v>
       </c>
-      <c r="AI23" t="n">
+      <c r="AX23" t="n">
         <v>-0.260091438547937</v>
       </c>
-      <c r="AJ23" t="n">
+      <c r="AY23" t="n">
         <v>4.258499458497695</v>
       </c>
-      <c r="AK23" t="n">
+      <c r="AZ23" t="n">
         <v>-1.977407815367054</v>
       </c>
     </row>
@@ -3117,105 +4182,150 @@
         <v>2.75</v>
       </c>
       <c r="D24" t="n">
+        <v>240.575712006407</v>
+      </c>
+      <c r="E24" t="n">
         <v>15.047480197663</v>
       </c>
-      <c r="E24" t="n">
+      <c r="F24" t="n">
+        <v>239.4938810497311</v>
+      </c>
+      <c r="G24" t="n">
         <v>17.7030786554864</v>
       </c>
-      <c r="F24" t="n">
+      <c r="H24" t="n">
+        <v>256.9980186509325</v>
+      </c>
+      <c r="I24" t="n">
         <v>2.691878663732648</v>
       </c>
-      <c r="G24" t="n">
+      <c r="J24" t="n">
+        <v>253.7966845517463</v>
+      </c>
+      <c r="K24" t="n">
         <v>5.406993162547438</v>
       </c>
-      <c r="H24" t="n">
+      <c r="L24" t="n">
+        <v>251.7364376402916</v>
+      </c>
+      <c r="M24" t="n">
         <v>11.80180488748753</v>
       </c>
-      <c r="I24" t="n">
+      <c r="N24" t="n">
+        <v>253.1458618370354</v>
+      </c>
+      <c r="O24" t="n">
         <v>16.99260988979475</v>
       </c>
-      <c r="J24" t="n">
+      <c r="P24" t="n">
+        <v>249.6862596865242</v>
+      </c>
+      <c r="Q24" t="n">
         <v>25.01688510813611</v>
       </c>
-      <c r="K24" t="n">
+      <c r="R24" t="n">
+        <v>210.3927784777702</v>
+      </c>
+      <c r="S24" t="n">
         <v>25.50218561862378</v>
       </c>
-      <c r="L24" t="n">
+      <c r="T24" t="n">
+        <v>205.693655994767</v>
+      </c>
+      <c r="U24" t="n">
         <v>17.61095608379824</v>
       </c>
-      <c r="M24" t="n">
+      <c r="V24" t="n">
+        <v>206.047389693294</v>
+      </c>
+      <c r="W24" t="n">
         <v>8.385990359258988</v>
       </c>
-      <c r="N24" t="n">
+      <c r="X24" t="n">
+        <v>193.9647701615138</v>
+      </c>
+      <c r="Y24" t="n">
         <v>10.94906448472476</v>
       </c>
-      <c r="O24" t="n">
+      <c r="Z24" t="n">
+        <v>195.3490605591037</v>
+      </c>
+      <c r="AA24" t="n">
         <v>0.9466861156707135</v>
       </c>
-      <c r="P24" t="n">
+      <c r="AB24" t="n">
+        <v>192.9487335766461</v>
+      </c>
+      <c r="AC24" t="n">
         <v>18.9976692199707</v>
       </c>
-      <c r="Q24" t="n">
+      <c r="AD24" t="n">
+        <v>162.5891914604404</v>
+      </c>
+      <c r="AE24" t="n">
         <v>31.49635588869135</v>
       </c>
-      <c r="R24" t="n">
+      <c r="AF24" t="n">
+        <v>132.0553094782728</v>
+      </c>
+      <c r="AG24" t="n">
         <v>46.11210028330485</v>
       </c>
-      <c r="S24" t="n">
+      <c r="AH24" t="n">
         <v>69.17904581724117</v>
       </c>
-      <c r="T24" t="n">
+      <c r="AI24" t="n">
         <v>75.85802588887006</v>
       </c>
-      <c r="U24" t="n">
+      <c r="AJ24" t="n">
         <v>147.0309825044826</v>
       </c>
-      <c r="V24" t="n">
+      <c r="AK24" t="n">
         <v>0.1947907268578311</v>
       </c>
-      <c r="W24" t="n">
+      <c r="AL24" t="n">
         <v>0.4179905915091236</v>
       </c>
-      <c r="X24" t="n">
+      <c r="AM24" t="n">
         <v>1.687424656347184</v>
       </c>
-      <c r="Y24" t="n">
+      <c r="AN24" t="n">
         <v>0.5642475599938228</v>
       </c>
-      <c r="Z24" t="n">
+      <c r="AO24" t="n">
         <v>1.515152183830318</v>
       </c>
-      <c r="AA24" t="n">
+      <c r="AP24" t="n">
         <v>0.5887412010355166</v>
       </c>
-      <c r="AB24" t="n">
+      <c r="AQ24" t="n">
         <v>2.092557342339913</v>
       </c>
-      <c r="AC24" t="n">
+      <c r="AR24" t="n">
         <v>0.01923219954713865</v>
       </c>
-      <c r="AD24" t="n">
+      <c r="AS24" t="n">
         <v>2.27064198635994</v>
       </c>
-      <c r="AE24" t="n">
+      <c r="AT24" t="n">
         <v>-0.0291539422163743</v>
       </c>
-      <c r="AF24" t="n">
+      <c r="AU24" t="n">
         <v>5.639502011107558</v>
       </c>
-      <c r="AG24" t="n">
+      <c r="AV24" t="n">
         <v>1.47315241254263</v>
       </c>
-      <c r="AH24" t="n">
+      <c r="AW24" t="n">
         <v>1.158941522161847</v>
       </c>
-      <c r="AI24" t="n">
+      <c r="AX24" t="n">
         <v>-3.011403508134501</v>
       </c>
-      <c r="AJ24" t="n">
+      <c r="AY24" t="n">
         <v>2.514277025835938</v>
       </c>
-      <c r="AK24" t="n">
+      <c r="AZ24" t="n">
         <v>-3.658853020641918</v>
       </c>
     </row>
@@ -3230,105 +4340,150 @@
         <v>2.75</v>
       </c>
       <c r="D25" t="n">
+        <v>228.6547979551321</v>
+      </c>
+      <c r="E25" t="n">
         <v>11.92343826835037</v>
       </c>
-      <c r="E25" t="n">
+      <c r="F25" t="n">
+        <v>256.4759109618394</v>
+      </c>
+      <c r="G25" t="n">
         <v>18.44986651806121</v>
       </c>
-      <c r="F25" t="n">
+      <c r="H25" t="n">
+        <v>253.4583795366558</v>
+      </c>
+      <c r="I25" t="n">
         <v>4.955518330242614</v>
       </c>
-      <c r="G25" t="n">
+      <c r="J25" t="n">
+        <v>251.1632792070402</v>
+      </c>
+      <c r="K25" t="n">
         <v>6.77190334238904</v>
       </c>
-      <c r="H25" t="n">
+      <c r="L25" t="n">
+        <v>253.6299303702429</v>
+      </c>
+      <c r="M25" t="n">
         <v>12.32998793852245</v>
       </c>
-      <c r="I25" t="n">
+      <c r="N25" t="n">
+        <v>254.7243628703745</v>
+      </c>
+      <c r="O25" t="n">
         <v>16.98564231818449</v>
       </c>
-      <c r="J25" t="n">
+      <c r="P25" t="n">
+        <v>247.861325994451</v>
+      </c>
+      <c r="Q25" t="n">
         <v>25.08869847507341</v>
       </c>
-      <c r="K25" t="n">
+      <c r="R25" t="n">
+        <v>213.077471104074</v>
+      </c>
+      <c r="S25" t="n">
         <v>25.87093309307775</v>
       </c>
-      <c r="L25" t="n">
+      <c r="T25" t="n">
+        <v>208.1679022903983</v>
+      </c>
+      <c r="U25" t="n">
         <v>17.96630764683933</v>
       </c>
-      <c r="M25" t="n">
+      <c r="V25" t="n">
+        <v>208.1719687644472</v>
+      </c>
+      <c r="W25" t="n">
         <v>8.703896001721105</v>
       </c>
-      <c r="N25" t="n">
+      <c r="X25" t="n">
+        <v>196.0659286654587</v>
+      </c>
+      <c r="Y25" t="n">
         <v>11.80459759759565</v>
       </c>
-      <c r="O25" t="n">
+      <c r="Z25" t="n">
+        <v>195.7527780363746</v>
+      </c>
+      <c r="AA25" t="n">
         <v>1.204411865126156</v>
       </c>
-      <c r="P25" t="n">
+      <c r="AB25" t="n">
+        <v>195.3647144297336</v>
+      </c>
+      <c r="AC25" t="n">
         <v>19.44925463791435</v>
       </c>
-      <c r="Q25" t="n">
+      <c r="AD25" t="n">
+        <v>165.2929503021511</v>
+      </c>
+      <c r="AE25" t="n">
         <v>30.77718197031224</v>
       </c>
-      <c r="R25" t="n">
+      <c r="AF25" t="n">
+        <v>135.1015095169662</v>
+      </c>
+      <c r="AG25" t="n">
         <v>44.27207446267419</v>
       </c>
-      <c r="S25" t="n">
+      <c r="AH25" t="n">
         <v>76.28780075086662</v>
       </c>
-      <c r="T25" t="n">
+      <c r="AI25" t="n">
         <v>75.56826445066841</v>
       </c>
-      <c r="U25" t="n">
+      <c r="AJ25" t="n">
         <v>148.1138739542072</v>
       </c>
-      <c r="V25" t="n">
+      <c r="AK25" t="n">
         <v>0.9356178290455067</v>
       </c>
-      <c r="W25" t="n">
+      <c r="AL25" t="n">
         <v>0.6621661972492288</v>
       </c>
-      <c r="X25" t="n">
+      <c r="AM25" t="n">
         <v>2.655327277826079</v>
       </c>
-      <c r="Y25" t="n">
+      <c r="AN25" t="n">
         <v>0.8289782713491028</v>
       </c>
-      <c r="Z25" t="n">
+      <c r="AO25" t="n">
         <v>2.632724393344092</v>
       </c>
-      <c r="AA25" t="n">
+      <c r="AP25" t="n">
         <v>0.7848112295705362</v>
       </c>
-      <c r="AB25" t="n">
+      <c r="AQ25" t="n">
         <v>2.19521091339436</v>
       </c>
-      <c r="AC25" t="n">
+      <c r="AR25" t="n">
         <v>0.005725723631841248</v>
       </c>
-      <c r="AD25" t="n">
+      <c r="AS25" t="n">
         <v>2.292216500491962</v>
       </c>
-      <c r="AE25" t="n">
+      <c r="AT25" t="n">
         <v>-0.141246606272163</v>
       </c>
-      <c r="AF25" t="n">
+      <c r="AU25" t="n">
         <v>8.607769908375927</v>
       </c>
-      <c r="AG25" t="n">
+      <c r="AV25" t="n">
         <v>1.913896031061286</v>
       </c>
-      <c r="AH25" t="n">
+      <c r="AW25" t="n">
         <v>-3.847605788863579</v>
       </c>
-      <c r="AI25" t="n">
+      <c r="AX25" t="n">
         <v>-4.057625306592195</v>
       </c>
-      <c r="AJ25" t="n">
+      <c r="AY25" t="n">
         <v>-4.026168971459761</v>
       </c>
-      <c r="AK25" t="n">
+      <c r="AZ25" t="n">
         <v>-4.739459769815207</v>
       </c>
     </row>
@@ -3343,105 +4498,150 @@
         <v>2.75</v>
       </c>
       <c r="D26" t="n">
+        <v>205.7171060010157</v>
+      </c>
+      <c r="E26" t="n">
         <v>17.09548767576826</v>
       </c>
-      <c r="E26" t="n">
+      <c r="F26" t="n">
+        <v>247.6779559270499</v>
+      </c>
+      <c r="G26" t="n">
         <v>19.23955450666711</v>
       </c>
-      <c r="F26" t="n">
+      <c r="H26" t="n">
+        <v>258.4613440941411</v>
+      </c>
+      <c r="I26" t="n">
         <v>2.1925594789762</v>
       </c>
-      <c r="G26" t="n">
+      <c r="J26" t="n">
+        <v>255.8458683127207</v>
+      </c>
+      <c r="K26" t="n">
         <v>5.49561284112592</v>
       </c>
-      <c r="H26" t="n">
+      <c r="L26" t="n">
+        <v>252.5277585848004</v>
+      </c>
+      <c r="M26" t="n">
         <v>12.54775574866762</v>
       </c>
-      <c r="I26" t="n">
+      <c r="N26" t="n">
+        <v>256.2534187808105</v>
+      </c>
+      <c r="O26" t="n">
         <v>17.43074342714134</v>
       </c>
-      <c r="J26" t="n">
+      <c r="P26" t="n">
+        <v>257.4382421131253</v>
+      </c>
+      <c r="Q26" t="n">
         <v>24.69154283510033</v>
       </c>
-      <c r="K26" t="n">
+      <c r="R26" t="n">
+        <v>215.5467645496342</v>
+      </c>
+      <c r="S26" t="n">
         <v>26.40235221132319</v>
       </c>
-      <c r="L26" t="n">
+      <c r="T26" t="n">
+        <v>210.7231694755825</v>
+      </c>
+      <c r="U26" t="n">
         <v>18.7584603086431</v>
       </c>
-      <c r="M26" t="n">
+      <c r="V26" t="n">
+        <v>211.9611620057559</v>
+      </c>
+      <c r="W26" t="n">
         <v>9.975508764280494</v>
       </c>
-      <c r="N26" t="n">
+      <c r="X26" t="n">
+        <v>200.1309862373569</v>
+      </c>
+      <c r="Y26" t="n">
         <v>13.12309630373691</v>
       </c>
-      <c r="O26" t="n">
+      <c r="Z26" t="n">
+        <v>197.4490816711534</v>
+      </c>
+      <c r="AA26" t="n">
         <v>2.238601995698098</v>
       </c>
-      <c r="P26" t="n">
+      <c r="AB26" t="n">
+        <v>197.7666668012633</v>
+      </c>
+      <c r="AC26" t="n">
         <v>19.9803795374877</v>
       </c>
-      <c r="Q26" t="n">
+      <c r="AD26" t="n">
+        <v>167.8237935330006</v>
+      </c>
+      <c r="AE26" t="n">
         <v>30.63365550751382</v>
       </c>
-      <c r="R26" t="n">
+      <c r="AF26" t="n">
+        <v>137.4281596630178</v>
+      </c>
+      <c r="AG26" t="n">
         <v>43.03779720414614</v>
       </c>
-      <c r="S26" t="n">
+      <c r="AH26" t="n">
         <v>88.92195269481878</v>
       </c>
-      <c r="T26" t="n">
+      <c r="AI26" t="n">
         <v>66.96609061004969</v>
       </c>
-      <c r="U26" t="n">
+      <c r="AJ26" t="n">
         <v>139.5461199534943</v>
       </c>
-      <c r="V26" t="n">
+      <c r="AK26" t="n">
         <v>1.656970402873154</v>
       </c>
-      <c r="W26" t="n">
+      <c r="AL26" t="n">
         <v>0.6739016965771394</v>
       </c>
-      <c r="X26" t="n">
+      <c r="AM26" t="n">
         <v>3.661775842626044</v>
       </c>
-      <c r="Y26" t="n">
+      <c r="AN26" t="n">
         <v>0.6945158995635068</v>
       </c>
-      <c r="Z26" t="n">
+      <c r="AO26" t="n">
         <v>3.400053031055643</v>
       </c>
-      <c r="AA26" t="n">
+      <c r="AP26" t="n">
         <v>0.7098488351132052</v>
       </c>
-      <c r="AB26" t="n">
+      <c r="AQ26" t="n">
         <v>2.273766622475707</v>
       </c>
-      <c r="AC26" t="n">
+      <c r="AR26" t="n">
         <v>0.124732822391167</v>
       </c>
-      <c r="AD26" t="n">
+      <c r="AS26" t="n">
         <v>2.133213797359603</v>
       </c>
-      <c r="AE26" t="n">
+      <c r="AT26" t="n">
         <v>-0.05270086281688169</v>
       </c>
-      <c r="AF26" t="n">
+      <c r="AU26" t="n">
         <v>9.867410926663648</v>
       </c>
-      <c r="AG26" t="n">
+      <c r="AV26" t="n">
         <v>0.2940000664839944</v>
       </c>
-      <c r="AH26" t="n">
+      <c r="AW26" t="n">
         <v>-8.254142958977457</v>
       </c>
-      <c r="AI26" t="n">
+      <c r="AX26" t="n">
         <v>-3.519604469541105</v>
       </c>
-      <c r="AJ26" t="n">
+      <c r="AY26" t="n">
         <v>-7.609851084150319</v>
       </c>
-      <c r="AK26" t="n">
+      <c r="AZ26" t="n">
         <v>-3.415011641588054</v>
       </c>
     </row>

</xml_diff>